<commit_message>
Notificacion se relaciona con Personal
</commit_message>
<xml_diff>
--- a/Datos/personal.xlsx
+++ b/Datos/personal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\Auxiliar\proyecto\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24AA00C8-0C11-4A39-9222-710F7F3CFD93}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F8D11C9-81C9-4C37-A083-E1554D82F278}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="1025">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="1026">
   <si>
     <t>Alquicira</t>
   </si>
@@ -3095,6 +3095,9 @@
   </si>
   <si>
     <t>ROLE_DOC</t>
+  </si>
+  <si>
+    <t>idhorario</t>
   </si>
 </sst>
 </file>
@@ -3982,10 +3985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J255"/>
+  <dimension ref="A1:K255"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3999,9 +4002,10 @@
     <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>507</v>
       </c>
@@ -4032,8 +4036,11 @@
       <c r="J1" s="1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4064,8 +4071,11 @@
       <c r="J2" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4096,8 +4106,11 @@
       <c r="J3" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4128,8 +4141,11 @@
       <c r="J4" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4160,8 +4176,11 @@
       <c r="J5" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4192,8 +4211,11 @@
       <c r="J6" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4224,8 +4246,11 @@
       <c r="J7" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4256,8 +4281,11 @@
       <c r="J8" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4288,8 +4316,11 @@
       <c r="J9" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4320,8 +4351,11 @@
       <c r="J10" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4352,8 +4386,11 @@
       <c r="J11" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4384,8 +4421,11 @@
       <c r="J12" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4416,8 +4456,11 @@
       <c r="J13" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4448,8 +4491,11 @@
       <c r="J14" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4480,8 +4526,11 @@
       <c r="J15" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4512,8 +4561,11 @@
       <c r="J16" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4544,8 +4596,11 @@
       <c r="J17" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4576,8 +4631,11 @@
       <c r="J18" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4608,8 +4666,11 @@
       <c r="J19" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4640,8 +4701,11 @@
       <c r="J20" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4672,8 +4736,11 @@
       <c r="J21" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4704,8 +4771,11 @@
       <c r="J22" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4736,8 +4806,11 @@
       <c r="J23" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4768,8 +4841,11 @@
       <c r="J24" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4800,8 +4876,11 @@
       <c r="J25" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4832,8 +4911,11 @@
       <c r="J26" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -4864,8 +4946,11 @@
       <c r="J27" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -4896,8 +4981,11 @@
       <c r="J28" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -4928,8 +5016,11 @@
       <c r="J29" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -4960,8 +5051,11 @@
       <c r="J30" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -4992,8 +5086,11 @@
       <c r="J31" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5024,8 +5121,11 @@
       <c r="J32" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5056,8 +5156,11 @@
       <c r="J33" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5088,8 +5191,11 @@
       <c r="J34" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5120,8 +5226,11 @@
       <c r="J35" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5152,8 +5261,11 @@
       <c r="J36" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5184,8 +5296,11 @@
       <c r="J37" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5216,8 +5331,11 @@
       <c r="J38" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -5248,8 +5366,11 @@
       <c r="J39" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -5280,8 +5401,11 @@
       <c r="J40" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -5312,8 +5436,11 @@
       <c r="J41" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -5344,8 +5471,11 @@
       <c r="J42" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -5376,8 +5506,11 @@
       <c r="J43" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -5408,8 +5541,11 @@
       <c r="J44" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -5440,8 +5576,11 @@
       <c r="J45" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -5472,8 +5611,11 @@
       <c r="J46" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -5504,8 +5646,11 @@
       <c r="J47" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -5536,8 +5681,11 @@
       <c r="J48" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -5568,8 +5716,11 @@
       <c r="J49" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -5600,8 +5751,11 @@
       <c r="J50" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -5632,8 +5786,11 @@
       <c r="J51" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -5664,8 +5821,11 @@
       <c r="J52" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -5696,8 +5856,11 @@
       <c r="J53" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -5728,8 +5891,11 @@
       <c r="J54" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -5760,8 +5926,11 @@
       <c r="J55" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -5792,8 +5961,11 @@
       <c r="J56" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -5824,8 +5996,11 @@
       <c r="J57" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -5856,8 +6031,11 @@
       <c r="J58" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -5888,8 +6066,11 @@
       <c r="J59" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -5920,8 +6101,11 @@
       <c r="J60" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -5952,8 +6136,11 @@
       <c r="J61" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -5984,8 +6171,11 @@
       <c r="J62" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -6016,8 +6206,11 @@
       <c r="J63" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -6048,8 +6241,11 @@
       <c r="J64" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -6080,8 +6276,11 @@
       <c r="J65" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -6112,8 +6311,11 @@
       <c r="J66" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -6144,8 +6346,11 @@
       <c r="J67" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -6176,8 +6381,11 @@
       <c r="J68" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -6208,8 +6416,11 @@
       <c r="J69" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -6240,8 +6451,11 @@
       <c r="J70" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -6272,8 +6486,11 @@
       <c r="J71" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -6304,8 +6521,11 @@
       <c r="J72" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -6336,8 +6556,11 @@
       <c r="J73" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -6368,8 +6591,11 @@
       <c r="J74" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -6400,8 +6626,11 @@
       <c r="J75" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -6432,8 +6661,11 @@
       <c r="J76" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -6464,8 +6696,11 @@
       <c r="J77" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -6496,8 +6731,11 @@
       <c r="J78" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -6528,8 +6766,11 @@
       <c r="J79" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -6560,8 +6801,11 @@
       <c r="J80" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -6592,8 +6836,11 @@
       <c r="J81" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -6624,8 +6871,11 @@
       <c r="J82" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -6656,8 +6906,11 @@
       <c r="J83" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -6688,8 +6941,11 @@
       <c r="J84" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -6720,8 +6976,11 @@
       <c r="J85" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -6752,8 +7011,11 @@
       <c r="J86" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -6784,8 +7046,11 @@
       <c r="J87" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -6816,8 +7081,11 @@
       <c r="J88" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -6848,8 +7116,11 @@
       <c r="J89" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -6880,8 +7151,11 @@
       <c r="J90" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -6912,8 +7186,11 @@
       <c r="J91" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -6944,8 +7221,11 @@
       <c r="J92" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -6976,8 +7256,11 @@
       <c r="J93" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -7008,8 +7291,11 @@
       <c r="J94" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -7040,8 +7326,11 @@
       <c r="J95" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -7072,8 +7361,11 @@
       <c r="J96" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -7104,8 +7396,11 @@
       <c r="J97" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -7136,8 +7431,11 @@
       <c r="J98" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -7168,8 +7466,11 @@
       <c r="J99" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -7200,8 +7501,11 @@
       <c r="J100" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -7232,8 +7536,11 @@
       <c r="J101" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -7264,8 +7571,11 @@
       <c r="J102" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -7296,8 +7606,11 @@
       <c r="J103" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -7328,8 +7641,11 @@
       <c r="J104" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -7360,8 +7676,11 @@
       <c r="J105" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -7392,8 +7711,11 @@
       <c r="J106" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -7424,8 +7746,11 @@
       <c r="J107" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -7456,8 +7781,11 @@
       <c r="J108" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -7488,8 +7816,11 @@
       <c r="J109" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -7520,8 +7851,11 @@
       <c r="J110" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -7552,8 +7886,11 @@
       <c r="J111" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -7584,8 +7921,11 @@
       <c r="J112" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -7616,8 +7956,11 @@
       <c r="J113" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -7648,8 +7991,11 @@
       <c r="J114" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -7680,8 +8026,11 @@
       <c r="J115" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -7712,8 +8061,11 @@
       <c r="J116" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -7744,8 +8096,11 @@
       <c r="J117" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -7776,8 +8131,11 @@
       <c r="J118" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -7808,8 +8166,11 @@
       <c r="J119" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -7840,8 +8201,11 @@
       <c r="J120" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -7872,8 +8236,11 @@
       <c r="J121" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -7904,8 +8271,11 @@
       <c r="J122" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -7936,8 +8306,11 @@
       <c r="J123" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -7968,8 +8341,11 @@
       <c r="J124" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -8000,8 +8376,11 @@
       <c r="J125" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -8032,8 +8411,11 @@
       <c r="J126" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -8064,8 +8446,11 @@
       <c r="J127" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -8096,8 +8481,11 @@
       <c r="J128" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -8128,8 +8516,11 @@
       <c r="J129" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -8160,8 +8551,11 @@
       <c r="J130" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -8192,8 +8586,11 @@
       <c r="J131" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K131">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -8224,8 +8621,11 @@
       <c r="J132" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -8256,8 +8656,11 @@
       <c r="J133" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -8288,8 +8691,11 @@
       <c r="J134" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -8320,8 +8726,11 @@
       <c r="J135" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -8352,8 +8761,11 @@
       <c r="J136" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -8384,8 +8796,11 @@
       <c r="J137" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -8416,8 +8831,11 @@
       <c r="J138" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -8448,8 +8866,11 @@
       <c r="J139" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -8480,8 +8901,11 @@
       <c r="J140" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -8512,8 +8936,11 @@
       <c r="J141" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K141">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -8544,8 +8971,11 @@
       <c r="J142" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -8576,8 +9006,11 @@
       <c r="J143" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K143">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -8608,8 +9041,11 @@
       <c r="J144" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -8640,8 +9076,11 @@
       <c r="J145" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -8672,8 +9111,11 @@
       <c r="J146" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K146">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -8704,8 +9146,11 @@
       <c r="J147" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -8736,8 +9181,11 @@
       <c r="J148" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -8768,8 +9216,11 @@
       <c r="J149" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -8800,8 +9251,11 @@
       <c r="J150" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -8832,8 +9286,11 @@
       <c r="J151" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -8864,8 +9321,11 @@
       <c r="J152" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -8896,8 +9356,11 @@
       <c r="J153" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -8928,8 +9391,11 @@
       <c r="J154" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -8960,8 +9426,11 @@
       <c r="J155" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -8992,8 +9461,11 @@
       <c r="J156" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K156">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -9024,8 +9496,11 @@
       <c r="J157" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -9056,8 +9531,11 @@
       <c r="J158" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K158">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -9088,8 +9566,11 @@
       <c r="J159" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K159">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -9120,8 +9601,11 @@
       <c r="J160" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K160">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -9152,8 +9636,11 @@
       <c r="J161" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K161">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -9184,8 +9671,11 @@
       <c r="J162" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K162">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -9216,8 +9706,11 @@
       <c r="J163" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K163">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -9248,8 +9741,11 @@
       <c r="J164" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K164">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -9280,8 +9776,11 @@
       <c r="J165" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K165">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -9312,8 +9811,11 @@
       <c r="J166" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K166">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -9344,8 +9846,11 @@
       <c r="J167" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K167">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -9376,8 +9881,11 @@
       <c r="J168" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K168">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -9408,8 +9916,11 @@
       <c r="J169" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K169">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -9440,8 +9951,11 @@
       <c r="J170" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K170">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -9472,8 +9986,11 @@
       <c r="J171" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K171">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -9504,8 +10021,11 @@
       <c r="J172" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K172">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -9536,8 +10056,11 @@
       <c r="J173" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K173">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -9568,8 +10091,11 @@
       <c r="J174" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K174">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -9600,8 +10126,11 @@
       <c r="J175" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K175">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -9632,8 +10161,11 @@
       <c r="J176" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K176">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -9664,8 +10196,11 @@
       <c r="J177" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -9696,8 +10231,11 @@
       <c r="J178" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K178">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -9728,8 +10266,11 @@
       <c r="J179" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K179">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -9760,8 +10301,11 @@
       <c r="J180" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K180">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -9792,8 +10336,11 @@
       <c r="J181" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K181">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -9824,8 +10371,11 @@
       <c r="J182" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K182">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -9856,8 +10406,11 @@
       <c r="J183" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K183">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -9888,8 +10441,11 @@
       <c r="J184" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K184">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -9920,8 +10476,11 @@
       <c r="J185" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K185">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -9952,8 +10511,11 @@
       <c r="J186" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K186">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -9984,8 +10546,11 @@
       <c r="J187" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K187">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -10016,8 +10581,11 @@
       <c r="J188" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K188">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -10048,8 +10616,11 @@
       <c r="J189" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K189">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -10080,8 +10651,11 @@
       <c r="J190" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K190">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -10112,8 +10686,11 @@
       <c r="J191" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K191">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -10144,8 +10721,11 @@
       <c r="J192" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K192">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -10176,8 +10756,11 @@
       <c r="J193" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K193">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -10208,8 +10791,11 @@
       <c r="J194" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K194">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -10240,8 +10826,11 @@
       <c r="J195" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K195">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -10272,8 +10861,11 @@
       <c r="J196" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K196">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -10304,8 +10896,11 @@
       <c r="J197" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K197">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -10336,8 +10931,11 @@
       <c r="J198" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K198">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -10368,8 +10966,11 @@
       <c r="J199" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K199">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -10400,8 +11001,11 @@
       <c r="J200" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K200">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -10432,8 +11036,11 @@
       <c r="J201" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K201">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -10464,8 +11071,11 @@
       <c r="J202" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K202">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -10496,8 +11106,11 @@
       <c r="J203" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K203">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -10528,8 +11141,11 @@
       <c r="J204" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K204">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -10560,8 +11176,11 @@
       <c r="J205" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K205">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -10592,8 +11211,11 @@
       <c r="J206" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K206">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -10624,8 +11246,11 @@
       <c r="J207" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K207">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -10656,8 +11281,11 @@
       <c r="J208" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K208">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -10688,8 +11316,11 @@
       <c r="J209" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K209">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -10720,8 +11351,11 @@
       <c r="J210" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K210">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -10752,8 +11386,11 @@
       <c r="J211" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K211">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -10784,8 +11421,11 @@
       <c r="J212" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K212">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -10816,8 +11456,11 @@
       <c r="J213" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K213">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -10848,8 +11491,11 @@
       <c r="J214" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K214">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -10880,8 +11526,11 @@
       <c r="J215" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K215">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -10912,8 +11561,11 @@
       <c r="J216" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -10944,8 +11596,11 @@
       <c r="J217" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K217">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -10976,8 +11631,11 @@
       <c r="J218" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K218">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -11008,8 +11666,11 @@
       <c r="J219" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K219">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -11040,8 +11701,11 @@
       <c r="J220" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K220">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -11072,8 +11736,11 @@
       <c r="J221" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K221">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -11104,8 +11771,11 @@
       <c r="J222" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K222">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -11136,8 +11806,11 @@
       <c r="J223" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K223">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -11168,8 +11841,11 @@
       <c r="J224" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K224">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -11200,8 +11876,11 @@
       <c r="J225" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K225">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -11232,8 +11911,11 @@
       <c r="J226" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K226">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -11264,8 +11946,11 @@
       <c r="J227" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K227">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -11296,8 +11981,11 @@
       <c r="J228" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K228">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>228</v>
       </c>
@@ -11328,8 +12016,11 @@
       <c r="J229" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K229">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -11360,8 +12051,11 @@
       <c r="J230" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K230">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>230</v>
       </c>
@@ -11392,8 +12086,11 @@
       <c r="J231" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K231">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>231</v>
       </c>
@@ -11424,8 +12121,11 @@
       <c r="J232" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K232">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>232</v>
       </c>
@@ -11456,8 +12156,11 @@
       <c r="J233" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K233">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>233</v>
       </c>
@@ -11488,8 +12191,11 @@
       <c r="J234" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K234">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>234</v>
       </c>
@@ -11520,8 +12226,11 @@
       <c r="J235" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K235">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>235</v>
       </c>
@@ -11552,8 +12261,11 @@
       <c r="J236" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K236">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>236</v>
       </c>
@@ -11584,8 +12296,11 @@
       <c r="J237" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K237">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>237</v>
       </c>
@@ -11616,8 +12331,11 @@
       <c r="J238" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K238">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>238</v>
       </c>
@@ -11648,8 +12366,11 @@
       <c r="J239" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K239">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -11680,8 +12401,11 @@
       <c r="J240" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K240">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>240</v>
       </c>
@@ -11712,8 +12436,11 @@
       <c r="J241" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K241">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>241</v>
       </c>
@@ -11744,8 +12471,11 @@
       <c r="J242" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K242">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>242</v>
       </c>
@@ -11776,8 +12506,11 @@
       <c r="J243" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K243">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>243</v>
       </c>
@@ -11808,8 +12541,11 @@
       <c r="J244" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K244">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>244</v>
       </c>
@@ -11840,8 +12576,11 @@
       <c r="J245" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K245">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>245</v>
       </c>
@@ -11872,8 +12611,11 @@
       <c r="J246" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K246">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>246</v>
       </c>
@@ -11904,8 +12646,11 @@
       <c r="J247" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K247">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>247</v>
       </c>
@@ -11936,8 +12681,11 @@
       <c r="J248" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K248">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>248</v>
       </c>
@@ -11968,8 +12716,11 @@
       <c r="J249" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K249">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>249</v>
       </c>
@@ -12000,8 +12751,11 @@
       <c r="J250" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K250">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>250</v>
       </c>
@@ -12032,8 +12786,11 @@
       <c r="J251" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K251">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>251</v>
       </c>
@@ -12064,8 +12821,11 @@
       <c r="J252" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K252">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>252</v>
       </c>
@@ -12096,8 +12856,11 @@
       <c r="J253" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K253">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>253</v>
       </c>
@@ -12128,8 +12891,11 @@
       <c r="J254" s="1" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K254">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>254</v>
       </c>
@@ -12159,6 +12925,9 @@
       </c>
       <c r="J255" s="1" t="s">
         <v>1024</v>
+      </c>
+      <c r="K255">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
algunos registros de PAEE y CH
</commit_message>
<xml_diff>
--- a/Datos/personal.xlsx
+++ b/Datos/personal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F8D11C9-81C9-4C37-A083-E1554D82F278}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1823F2E7-1F3E-4D36-8B4C-A8BFCADC7D8E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="1042">
   <si>
     <t>Alquicira</t>
   </si>
@@ -3098,6 +3098,54 @@
   </si>
   <si>
     <t>idhorario</t>
+  </si>
+  <si>
+    <t>00000269</t>
+  </si>
+  <si>
+    <t>ROLE_PAEE</t>
+  </si>
+  <si>
+    <t>00000270</t>
+  </si>
+  <si>
+    <t>Vazquez</t>
+  </si>
+  <si>
+    <t>130001</t>
+  </si>
+  <si>
+    <t>130002</t>
+  </si>
+  <si>
+    <t>00000271</t>
+  </si>
+  <si>
+    <t>Nuñez</t>
+  </si>
+  <si>
+    <t>00000272</t>
+  </si>
+  <si>
+    <t>00000273</t>
+  </si>
+  <si>
+    <t>Camacho</t>
+  </si>
+  <si>
+    <t>ROLE_CH</t>
+  </si>
+  <si>
+    <t>00000274</t>
+  </si>
+  <si>
+    <t>Tania</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Sarabia</t>
   </si>
 </sst>
 </file>
@@ -3985,10 +4033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K255"/>
+  <dimension ref="A1:K261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="K262" sqref="K262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12930,6 +12978,216 @@
         <v>5</v>
       </c>
     </row>
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
+        <v>255</v>
+      </c>
+      <c r="B256" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F256" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G256" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H256" s="3" t="s">
+        <v>1030</v>
+      </c>
+      <c r="I256" s="1">
+        <v>13</v>
+      </c>
+      <c r="J256" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="K256">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A257" s="1">
+        <v>256</v>
+      </c>
+      <c r="B257" s="3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G257" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H257" s="3" t="s">
+        <v>1031</v>
+      </c>
+      <c r="I257" s="1">
+        <v>13</v>
+      </c>
+      <c r="J257" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="K257">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A258" s="1">
+        <v>257</v>
+      </c>
+      <c r="B258" s="3" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D258" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F258" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G258" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H258">
+        <v>130003</v>
+      </c>
+      <c r="I258" s="1">
+        <v>13</v>
+      </c>
+      <c r="J258" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="K258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A259" s="1">
+        <v>258</v>
+      </c>
+      <c r="B259" s="3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D259" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F259" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G259" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H259">
+        <v>170001</v>
+      </c>
+      <c r="I259" s="1">
+        <v>17</v>
+      </c>
+      <c r="J259" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="K259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A260" s="1">
+        <v>259</v>
+      </c>
+      <c r="B260" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D260" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="F260" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="G260" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H260">
+        <v>190001</v>
+      </c>
+      <c r="I260" s="1">
+        <v>19</v>
+      </c>
+      <c r="J260" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="K260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A261" s="1">
+        <v>260</v>
+      </c>
+      <c r="B261" s="3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F261" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="G261" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H261">
+        <v>190002</v>
+      </c>
+      <c r="I261" s="1">
+        <v>19</v>
+      </c>
+      <c r="J261" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="K261">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
estaban mal los num de tarjeta en personal
</commit_message>
<xml_diff>
--- a/Datos/personal.xlsx
+++ b/Datos/personal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD5B59DC-4548-47B2-9758-3CB37DD46584}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605E026E-2202-4189-991B-BC098DC1DF6A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="789">
   <si>
     <t>idempleado</t>
   </si>
@@ -1601,6 +1601,792 @@
   </si>
   <si>
     <t>Alemán</t>
+  </si>
+  <si>
+    <t>020001</t>
+  </si>
+  <si>
+    <t>020002</t>
+  </si>
+  <si>
+    <t>020003</t>
+  </si>
+  <si>
+    <t>020004</t>
+  </si>
+  <si>
+    <t>020005</t>
+  </si>
+  <si>
+    <t>020006</t>
+  </si>
+  <si>
+    <t>020007</t>
+  </si>
+  <si>
+    <t>020008</t>
+  </si>
+  <si>
+    <t>020009</t>
+  </si>
+  <si>
+    <t>020010</t>
+  </si>
+  <si>
+    <t>020011</t>
+  </si>
+  <si>
+    <t>020012</t>
+  </si>
+  <si>
+    <t>020013</t>
+  </si>
+  <si>
+    <t>020014</t>
+  </si>
+  <si>
+    <t>020015</t>
+  </si>
+  <si>
+    <t>020016</t>
+  </si>
+  <si>
+    <t>020017</t>
+  </si>
+  <si>
+    <t>020018</t>
+  </si>
+  <si>
+    <t>020019</t>
+  </si>
+  <si>
+    <t>020020</t>
+  </si>
+  <si>
+    <t>020021</t>
+  </si>
+  <si>
+    <t>020022</t>
+  </si>
+  <si>
+    <t>020023</t>
+  </si>
+  <si>
+    <t>020024</t>
+  </si>
+  <si>
+    <t>020025</t>
+  </si>
+  <si>
+    <t>020026</t>
+  </si>
+  <si>
+    <t>020027</t>
+  </si>
+  <si>
+    <t>020028</t>
+  </si>
+  <si>
+    <t>020029</t>
+  </si>
+  <si>
+    <t>020030</t>
+  </si>
+  <si>
+    <t>020031</t>
+  </si>
+  <si>
+    <t>020032</t>
+  </si>
+  <si>
+    <t>020033</t>
+  </si>
+  <si>
+    <t>020034</t>
+  </si>
+  <si>
+    <t>020035</t>
+  </si>
+  <si>
+    <t>020036</t>
+  </si>
+  <si>
+    <t>050001</t>
+  </si>
+  <si>
+    <t>050002</t>
+  </si>
+  <si>
+    <t>050003</t>
+  </si>
+  <si>
+    <t>050004</t>
+  </si>
+  <si>
+    <t>050005</t>
+  </si>
+  <si>
+    <t>050006</t>
+  </si>
+  <si>
+    <t>050007</t>
+  </si>
+  <si>
+    <t>050008</t>
+  </si>
+  <si>
+    <t>050009</t>
+  </si>
+  <si>
+    <t>050010</t>
+  </si>
+  <si>
+    <t>050011</t>
+  </si>
+  <si>
+    <t>050012</t>
+  </si>
+  <si>
+    <t>050013</t>
+  </si>
+  <si>
+    <t>050014</t>
+  </si>
+  <si>
+    <t>050015</t>
+  </si>
+  <si>
+    <t>050016</t>
+  </si>
+  <si>
+    <t>050017</t>
+  </si>
+  <si>
+    <t>050018</t>
+  </si>
+  <si>
+    <t>050019</t>
+  </si>
+  <si>
+    <t>050020</t>
+  </si>
+  <si>
+    <t>070001</t>
+  </si>
+  <si>
+    <t>070002</t>
+  </si>
+  <si>
+    <t>070003</t>
+  </si>
+  <si>
+    <t>070004</t>
+  </si>
+  <si>
+    <t>070005</t>
+  </si>
+  <si>
+    <t>070006</t>
+  </si>
+  <si>
+    <t>070007</t>
+  </si>
+  <si>
+    <t>070008</t>
+  </si>
+  <si>
+    <t>070009</t>
+  </si>
+  <si>
+    <t>070010</t>
+  </si>
+  <si>
+    <t>070011</t>
+  </si>
+  <si>
+    <t>070012</t>
+  </si>
+  <si>
+    <t>070013</t>
+  </si>
+  <si>
+    <t>070014</t>
+  </si>
+  <si>
+    <t>070015</t>
+  </si>
+  <si>
+    <t>070016</t>
+  </si>
+  <si>
+    <t>070017</t>
+  </si>
+  <si>
+    <t>070018</t>
+  </si>
+  <si>
+    <t>070019</t>
+  </si>
+  <si>
+    <t>070020</t>
+  </si>
+  <si>
+    <t>070021</t>
+  </si>
+  <si>
+    <t>070022</t>
+  </si>
+  <si>
+    <t>070023</t>
+  </si>
+  <si>
+    <t>070024</t>
+  </si>
+  <si>
+    <t>070025</t>
+  </si>
+  <si>
+    <t>070026</t>
+  </si>
+  <si>
+    <t>070027</t>
+  </si>
+  <si>
+    <t>070028</t>
+  </si>
+  <si>
+    <t>070029</t>
+  </si>
+  <si>
+    <t>070030</t>
+  </si>
+  <si>
+    <t>070031</t>
+  </si>
+  <si>
+    <t>070032</t>
+  </si>
+  <si>
+    <t>070033</t>
+  </si>
+  <si>
+    <t>070034</t>
+  </si>
+  <si>
+    <t>070035</t>
+  </si>
+  <si>
+    <t>070036</t>
+  </si>
+  <si>
+    <t>070037</t>
+  </si>
+  <si>
+    <t>070038</t>
+  </si>
+  <si>
+    <t>070039</t>
+  </si>
+  <si>
+    <t>070040</t>
+  </si>
+  <si>
+    <t>070041</t>
+  </si>
+  <si>
+    <t>070042</t>
+  </si>
+  <si>
+    <t>070043</t>
+  </si>
+  <si>
+    <t>070044</t>
+  </si>
+  <si>
+    <t>070045</t>
+  </si>
+  <si>
+    <t>070046</t>
+  </si>
+  <si>
+    <t>070047</t>
+  </si>
+  <si>
+    <t>070048</t>
+  </si>
+  <si>
+    <t>070049</t>
+  </si>
+  <si>
+    <t>070050</t>
+  </si>
+  <si>
+    <t>070051</t>
+  </si>
+  <si>
+    <t>060001</t>
+  </si>
+  <si>
+    <t>060002</t>
+  </si>
+  <si>
+    <t>060003</t>
+  </si>
+  <si>
+    <t>060004</t>
+  </si>
+  <si>
+    <t>060005</t>
+  </si>
+  <si>
+    <t>060006</t>
+  </si>
+  <si>
+    <t>060007</t>
+  </si>
+  <si>
+    <t>060008</t>
+  </si>
+  <si>
+    <t>060009</t>
+  </si>
+  <si>
+    <t>060010</t>
+  </si>
+  <si>
+    <t>060011</t>
+  </si>
+  <si>
+    <t>060012</t>
+  </si>
+  <si>
+    <t>060013</t>
+  </si>
+  <si>
+    <t>060014</t>
+  </si>
+  <si>
+    <t>060015</t>
+  </si>
+  <si>
+    <t>060016</t>
+  </si>
+  <si>
+    <t>060017</t>
+  </si>
+  <si>
+    <t>060018</t>
+  </si>
+  <si>
+    <t>060019</t>
+  </si>
+  <si>
+    <t>060020</t>
+  </si>
+  <si>
+    <t>060021</t>
+  </si>
+  <si>
+    <t>060022</t>
+  </si>
+  <si>
+    <t>060023</t>
+  </si>
+  <si>
+    <t>060024</t>
+  </si>
+  <si>
+    <t>060025</t>
+  </si>
+  <si>
+    <t>060026</t>
+  </si>
+  <si>
+    <t>060027</t>
+  </si>
+  <si>
+    <t>060028</t>
+  </si>
+  <si>
+    <t>060029</t>
+  </si>
+  <si>
+    <t>060030</t>
+  </si>
+  <si>
+    <t>060031</t>
+  </si>
+  <si>
+    <t>060032</t>
+  </si>
+  <si>
+    <t>060033</t>
+  </si>
+  <si>
+    <t>060034</t>
+  </si>
+  <si>
+    <t>060035</t>
+  </si>
+  <si>
+    <t>060036</t>
+  </si>
+  <si>
+    <t>060037</t>
+  </si>
+  <si>
+    <t>060038</t>
+  </si>
+  <si>
+    <t>060039</t>
+  </si>
+  <si>
+    <t>060040</t>
+  </si>
+  <si>
+    <t>060041</t>
+  </si>
+  <si>
+    <t>060042</t>
+  </si>
+  <si>
+    <t>060043</t>
+  </si>
+  <si>
+    <t>060044</t>
+  </si>
+  <si>
+    <t>060045</t>
+  </si>
+  <si>
+    <t>060046</t>
+  </si>
+  <si>
+    <t>060047</t>
+  </si>
+  <si>
+    <t>060048</t>
+  </si>
+  <si>
+    <t>060049</t>
+  </si>
+  <si>
+    <t>060050</t>
+  </si>
+  <si>
+    <t>060051</t>
+  </si>
+  <si>
+    <t>060052</t>
+  </si>
+  <si>
+    <t>060053</t>
+  </si>
+  <si>
+    <t>060054</t>
+  </si>
+  <si>
+    <t>060055</t>
+  </si>
+  <si>
+    <t>060056</t>
+  </si>
+  <si>
+    <t>060057</t>
+  </si>
+  <si>
+    <t>060058</t>
+  </si>
+  <si>
+    <t>060059</t>
+  </si>
+  <si>
+    <t>060060</t>
+  </si>
+  <si>
+    <t>060061</t>
+  </si>
+  <si>
+    <t>060062</t>
+  </si>
+  <si>
+    <t>060063</t>
+  </si>
+  <si>
+    <t>060064</t>
+  </si>
+  <si>
+    <t>060065</t>
+  </si>
+  <si>
+    <t>060066</t>
+  </si>
+  <si>
+    <t>060067</t>
+  </si>
+  <si>
+    <t>060068</t>
+  </si>
+  <si>
+    <t>060069</t>
+  </si>
+  <si>
+    <t>060070</t>
+  </si>
+  <si>
+    <t>060071</t>
+  </si>
+  <si>
+    <t>060072</t>
+  </si>
+  <si>
+    <t>060073</t>
+  </si>
+  <si>
+    <t>060074</t>
+  </si>
+  <si>
+    <t>060075</t>
+  </si>
+  <si>
+    <t>060076</t>
+  </si>
+  <si>
+    <t>060077</t>
+  </si>
+  <si>
+    <t>060078</t>
+  </si>
+  <si>
+    <t>060079</t>
+  </si>
+  <si>
+    <t>060080</t>
+  </si>
+  <si>
+    <t>060081</t>
+  </si>
+  <si>
+    <t>060082</t>
+  </si>
+  <si>
+    <t>060083</t>
+  </si>
+  <si>
+    <t>060084</t>
+  </si>
+  <si>
+    <t>060085</t>
+  </si>
+  <si>
+    <t>060086</t>
+  </si>
+  <si>
+    <t>060087</t>
+  </si>
+  <si>
+    <t>060088</t>
+  </si>
+  <si>
+    <t>060089</t>
+  </si>
+  <si>
+    <t>060090</t>
+  </si>
+  <si>
+    <t>060091</t>
+  </si>
+  <si>
+    <t>060092</t>
+  </si>
+  <si>
+    <t>060093</t>
+  </si>
+  <si>
+    <t>060094</t>
+  </si>
+  <si>
+    <t>060095</t>
+  </si>
+  <si>
+    <t>060096</t>
+  </si>
+  <si>
+    <t>060097</t>
+  </si>
+  <si>
+    <t>080001</t>
+  </si>
+  <si>
+    <t>080002</t>
+  </si>
+  <si>
+    <t>080003</t>
+  </si>
+  <si>
+    <t>080004</t>
+  </si>
+  <si>
+    <t>080005</t>
+  </si>
+  <si>
+    <t>080006</t>
+  </si>
+  <si>
+    <t>080007</t>
+  </si>
+  <si>
+    <t>080008</t>
+  </si>
+  <si>
+    <t>080009</t>
+  </si>
+  <si>
+    <t>080010</t>
+  </si>
+  <si>
+    <t>080011</t>
+  </si>
+  <si>
+    <t>080012</t>
+  </si>
+  <si>
+    <t>080013</t>
+  </si>
+  <si>
+    <t>080014</t>
+  </si>
+  <si>
+    <t>080015</t>
+  </si>
+  <si>
+    <t>080016</t>
+  </si>
+  <si>
+    <t>080017</t>
+  </si>
+  <si>
+    <t>080018</t>
+  </si>
+  <si>
+    <t>080019</t>
+  </si>
+  <si>
+    <t>080020</t>
+  </si>
+  <si>
+    <t>080021</t>
+  </si>
+  <si>
+    <t>080022</t>
+  </si>
+  <si>
+    <t>080023</t>
+  </si>
+  <si>
+    <t>080024</t>
+  </si>
+  <si>
+    <t>080025</t>
+  </si>
+  <si>
+    <t>080026</t>
+  </si>
+  <si>
+    <t>010001</t>
+  </si>
+  <si>
+    <t>010002</t>
+  </si>
+  <si>
+    <t>010003</t>
+  </si>
+  <si>
+    <t>010004</t>
+  </si>
+  <si>
+    <t>090152</t>
+  </si>
+  <si>
+    <t>090153</t>
+  </si>
+  <si>
+    <t>090124</t>
+  </si>
+  <si>
+    <t>090125</t>
+  </si>
+  <si>
+    <t>090126</t>
+  </si>
+  <si>
+    <t>090127</t>
+  </si>
+  <si>
+    <t>090128</t>
+  </si>
+  <si>
+    <t>090129</t>
+  </si>
+  <si>
+    <t>090130</t>
+  </si>
+  <si>
+    <t>090131</t>
+  </si>
+  <si>
+    <t>090132</t>
+  </si>
+  <si>
+    <t>090133</t>
+  </si>
+  <si>
+    <t>090134</t>
+  </si>
+  <si>
+    <t>090135</t>
+  </si>
+  <si>
+    <t>090136</t>
+  </si>
+  <si>
+    <t>090137</t>
+  </si>
+  <si>
+    <t>090138</t>
+  </si>
+  <si>
+    <t>090139</t>
+  </si>
+  <si>
+    <t>090140</t>
+  </si>
+  <si>
+    <t>090141</t>
+  </si>
+  <si>
+    <t>090142</t>
+  </si>
+  <si>
+    <t>090143</t>
+  </si>
+  <si>
+    <t>090144</t>
+  </si>
+  <si>
+    <t>090145</t>
+  </si>
+  <si>
+    <t>090146</t>
+  </si>
+  <si>
+    <t>090147</t>
+  </si>
+  <si>
+    <t>Itzel</t>
+  </si>
+  <si>
+    <t>090154</t>
   </si>
 </sst>
 </file>
@@ -2084,9 +2870,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -2444,10 +3233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L261"/>
+  <dimension ref="A1:L262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="H235" sqref="H235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2527,8 +3316,8 @@
       <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1">
-        <v>20001</v>
+      <c r="I2" s="2" t="s">
+        <v>527</v>
       </c>
       <c r="J2" s="1">
         <v>2</v>
@@ -2565,8 +3354,8 @@
       <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1">
-        <v>20002</v>
+      <c r="I3" s="2" t="s">
+        <v>528</v>
       </c>
       <c r="J3" s="1">
         <v>2</v>
@@ -2603,8 +3392,8 @@
       <c r="H4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="1">
-        <v>20003</v>
+      <c r="I4" s="2" t="s">
+        <v>529</v>
       </c>
       <c r="J4" s="1">
         <v>2</v>
@@ -2641,8 +3430,8 @@
       <c r="H5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="1">
-        <v>20004</v>
+      <c r="I5" s="2" t="s">
+        <v>530</v>
       </c>
       <c r="J5" s="1">
         <v>2</v>
@@ -2679,8 +3468,8 @@
       <c r="H6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="1">
-        <v>20005</v>
+      <c r="I6" s="2" t="s">
+        <v>531</v>
       </c>
       <c r="J6" s="1">
         <v>2</v>
@@ -2717,8 +3506,8 @@
       <c r="H7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="1">
-        <v>20006</v>
+      <c r="I7" s="2" t="s">
+        <v>532</v>
       </c>
       <c r="J7" s="1">
         <v>2</v>
@@ -2755,8 +3544,8 @@
       <c r="H8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="1">
-        <v>20007</v>
+      <c r="I8" s="2" t="s">
+        <v>533</v>
       </c>
       <c r="J8" s="1">
         <v>2</v>
@@ -2793,8 +3582,8 @@
       <c r="H9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="1">
-        <v>20008</v>
+      <c r="I9" s="2" t="s">
+        <v>534</v>
       </c>
       <c r="J9" s="1">
         <v>2</v>
@@ -2831,8 +3620,8 @@
       <c r="H10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="1">
-        <v>20009</v>
+      <c r="I10" s="2" t="s">
+        <v>535</v>
       </c>
       <c r="J10" s="1">
         <v>2</v>
@@ -2869,8 +3658,8 @@
       <c r="H11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="1">
-        <v>20010</v>
+      <c r="I11" s="2" t="s">
+        <v>536</v>
       </c>
       <c r="J11" s="1">
         <v>2</v>
@@ -2907,8 +3696,8 @@
       <c r="H12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="1">
-        <v>20011</v>
+      <c r="I12" s="2" t="s">
+        <v>537</v>
       </c>
       <c r="J12" s="1">
         <v>2</v>
@@ -2945,8 +3734,8 @@
       <c r="H13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="1">
-        <v>20012</v>
+      <c r="I13" s="2" t="s">
+        <v>538</v>
       </c>
       <c r="J13" s="1">
         <v>2</v>
@@ -2983,8 +3772,8 @@
       <c r="H14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="1">
-        <v>20013</v>
+      <c r="I14" s="2" t="s">
+        <v>539</v>
       </c>
       <c r="J14" s="1">
         <v>2</v>
@@ -3021,8 +3810,8 @@
       <c r="H15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="1">
-        <v>20014</v>
+      <c r="I15" s="2" t="s">
+        <v>540</v>
       </c>
       <c r="J15" s="1">
         <v>2</v>
@@ -3059,8 +3848,8 @@
       <c r="H16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I16" s="1">
-        <v>20015</v>
+      <c r="I16" s="2" t="s">
+        <v>541</v>
       </c>
       <c r="J16" s="1">
         <v>2</v>
@@ -3097,8 +3886,8 @@
       <c r="H17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I17" s="1">
-        <v>20016</v>
+      <c r="I17" s="2" t="s">
+        <v>542</v>
       </c>
       <c r="J17" s="1">
         <v>2</v>
@@ -3135,8 +3924,8 @@
       <c r="H18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="1">
-        <v>20017</v>
+      <c r="I18" s="2" t="s">
+        <v>543</v>
       </c>
       <c r="J18" s="1">
         <v>2</v>
@@ -3173,8 +3962,8 @@
       <c r="H19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I19" s="1">
-        <v>20018</v>
+      <c r="I19" s="2" t="s">
+        <v>544</v>
       </c>
       <c r="J19" s="1">
         <v>2</v>
@@ -3211,8 +4000,8 @@
       <c r="H20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="1">
-        <v>20019</v>
+      <c r="I20" s="2" t="s">
+        <v>545</v>
       </c>
       <c r="J20" s="1">
         <v>2</v>
@@ -3249,8 +4038,8 @@
       <c r="H21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I21" s="1">
-        <v>20020</v>
+      <c r="I21" s="2" t="s">
+        <v>546</v>
       </c>
       <c r="J21" s="1">
         <v>2</v>
@@ -3287,8 +4076,8 @@
       <c r="H22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I22" s="1">
-        <v>20021</v>
+      <c r="I22" s="2" t="s">
+        <v>547</v>
       </c>
       <c r="J22" s="1">
         <v>2</v>
@@ -3325,8 +4114,8 @@
       <c r="H23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I23" s="1">
-        <v>20022</v>
+      <c r="I23" s="2" t="s">
+        <v>548</v>
       </c>
       <c r="J23" s="1">
         <v>2</v>
@@ -3363,8 +4152,8 @@
       <c r="H24" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="1">
-        <v>20023</v>
+      <c r="I24" s="2" t="s">
+        <v>549</v>
       </c>
       <c r="J24" s="1">
         <v>2</v>
@@ -3401,8 +4190,8 @@
       <c r="H25" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I25" s="1">
-        <v>20024</v>
+      <c r="I25" s="2" t="s">
+        <v>550</v>
       </c>
       <c r="J25" s="1">
         <v>2</v>
@@ -3439,8 +4228,8 @@
       <c r="H26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I26" s="1">
-        <v>20025</v>
+      <c r="I26" s="2" t="s">
+        <v>551</v>
       </c>
       <c r="J26" s="1">
         <v>2</v>
@@ -3477,8 +4266,8 @@
       <c r="H27" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I27" s="1">
-        <v>20026</v>
+      <c r="I27" s="2" t="s">
+        <v>552</v>
       </c>
       <c r="J27" s="1">
         <v>2</v>
@@ -3515,8 +4304,8 @@
       <c r="H28" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I28" s="1">
-        <v>20027</v>
+      <c r="I28" s="2" t="s">
+        <v>553</v>
       </c>
       <c r="J28" s="1">
         <v>2</v>
@@ -3553,8 +4342,8 @@
       <c r="H29" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I29" s="1">
-        <v>20028</v>
+      <c r="I29" s="2" t="s">
+        <v>554</v>
       </c>
       <c r="J29" s="1">
         <v>2</v>
@@ -3591,8 +4380,8 @@
       <c r="H30" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I30" s="1">
-        <v>20029</v>
+      <c r="I30" s="2" t="s">
+        <v>555</v>
       </c>
       <c r="J30" s="1">
         <v>2</v>
@@ -3629,8 +4418,8 @@
       <c r="H31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I31" s="1">
-        <v>20030</v>
+      <c r="I31" s="2" t="s">
+        <v>556</v>
       </c>
       <c r="J31" s="1">
         <v>2</v>
@@ -3667,8 +4456,8 @@
       <c r="H32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I32" s="1">
-        <v>20031</v>
+      <c r="I32" s="2" t="s">
+        <v>557</v>
       </c>
       <c r="J32" s="1">
         <v>2</v>
@@ -3705,8 +4494,8 @@
       <c r="H33" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I33" s="1">
-        <v>20032</v>
+      <c r="I33" s="2" t="s">
+        <v>558</v>
       </c>
       <c r="J33" s="1">
         <v>2</v>
@@ -3743,8 +4532,8 @@
       <c r="H34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="I34" s="1">
-        <v>20033</v>
+      <c r="I34" s="2" t="s">
+        <v>559</v>
       </c>
       <c r="J34" s="1">
         <v>2</v>
@@ -3781,8 +4570,8 @@
       <c r="H35" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I35" s="1">
-        <v>20034</v>
+      <c r="I35" s="2" t="s">
+        <v>560</v>
       </c>
       <c r="J35" s="1">
         <v>2</v>
@@ -3819,8 +4608,8 @@
       <c r="H36" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="I36" s="1">
-        <v>20035</v>
+      <c r="I36" s="2" t="s">
+        <v>561</v>
       </c>
       <c r="J36" s="1">
         <v>2</v>
@@ -3857,8 +4646,8 @@
       <c r="H37" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I37" s="1">
-        <v>20036</v>
+      <c r="I37" s="2" t="s">
+        <v>562</v>
       </c>
       <c r="J37" s="1">
         <v>2</v>
@@ -3895,8 +4684,8 @@
       <c r="H38" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I38" s="1">
-        <v>50001</v>
+      <c r="I38" s="2" t="s">
+        <v>563</v>
       </c>
       <c r="J38" s="1">
         <v>5</v>
@@ -3933,8 +4722,8 @@
       <c r="H39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I39" s="1">
-        <v>50002</v>
+      <c r="I39" s="2" t="s">
+        <v>564</v>
       </c>
       <c r="J39" s="1">
         <v>5</v>
@@ -3971,8 +4760,8 @@
       <c r="H40" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I40" s="1">
-        <v>50003</v>
+      <c r="I40" s="2" t="s">
+        <v>565</v>
       </c>
       <c r="J40" s="1">
         <v>5</v>
@@ -4009,8 +4798,8 @@
       <c r="H41" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I41" s="1">
-        <v>50004</v>
+      <c r="I41" s="2" t="s">
+        <v>566</v>
       </c>
       <c r="J41" s="1">
         <v>5</v>
@@ -4047,8 +4836,8 @@
       <c r="H42" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I42" s="1">
-        <v>50005</v>
+      <c r="I42" s="2" t="s">
+        <v>567</v>
       </c>
       <c r="J42" s="1">
         <v>5</v>
@@ -4085,8 +4874,8 @@
       <c r="H43" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I43" s="1">
-        <v>50006</v>
+      <c r="I43" s="2" t="s">
+        <v>568</v>
       </c>
       <c r="J43" s="1">
         <v>5</v>
@@ -4123,8 +4912,8 @@
       <c r="H44" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I44" s="1">
-        <v>50007</v>
+      <c r="I44" s="2" t="s">
+        <v>569</v>
       </c>
       <c r="J44" s="1">
         <v>5</v>
@@ -4161,8 +4950,8 @@
       <c r="H45" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I45" s="1">
-        <v>50008</v>
+      <c r="I45" s="2" t="s">
+        <v>570</v>
       </c>
       <c r="J45" s="1">
         <v>5</v>
@@ -4199,8 +4988,8 @@
       <c r="H46" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I46" s="1">
-        <v>50009</v>
+      <c r="I46" s="2" t="s">
+        <v>571</v>
       </c>
       <c r="J46" s="1">
         <v>5</v>
@@ -4237,8 +5026,8 @@
       <c r="H47" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I47" s="1">
-        <v>50010</v>
+      <c r="I47" s="2" t="s">
+        <v>572</v>
       </c>
       <c r="J47" s="1">
         <v>5</v>
@@ -4275,8 +5064,8 @@
       <c r="H48" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I48" s="1">
-        <v>50011</v>
+      <c r="I48" s="2" t="s">
+        <v>573</v>
       </c>
       <c r="J48" s="1">
         <v>5</v>
@@ -4313,8 +5102,8 @@
       <c r="H49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I49" s="1">
-        <v>50012</v>
+      <c r="I49" s="2" t="s">
+        <v>574</v>
       </c>
       <c r="J49" s="1">
         <v>5</v>
@@ -4351,8 +5140,8 @@
       <c r="H50" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I50" s="1">
-        <v>50013</v>
+      <c r="I50" s="2" t="s">
+        <v>575</v>
       </c>
       <c r="J50" s="1">
         <v>5</v>
@@ -4389,8 +5178,8 @@
       <c r="H51" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I51" s="1">
-        <v>50014</v>
+      <c r="I51" s="2" t="s">
+        <v>576</v>
       </c>
       <c r="J51" s="1">
         <v>5</v>
@@ -4427,8 +5216,8 @@
       <c r="H52" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I52" s="1">
-        <v>50015</v>
+      <c r="I52" s="2" t="s">
+        <v>577</v>
       </c>
       <c r="J52" s="1">
         <v>5</v>
@@ -4465,8 +5254,8 @@
       <c r="H53" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I53" s="1">
-        <v>50016</v>
+      <c r="I53" s="2" t="s">
+        <v>578</v>
       </c>
       <c r="J53" s="1">
         <v>5</v>
@@ -4503,8 +5292,8 @@
       <c r="H54" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="I54" s="1">
-        <v>50017</v>
+      <c r="I54" s="2" t="s">
+        <v>579</v>
       </c>
       <c r="J54" s="1">
         <v>5</v>
@@ -4541,8 +5330,8 @@
       <c r="H55" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I55" s="1">
-        <v>50018</v>
+      <c r="I55" s="2" t="s">
+        <v>580</v>
       </c>
       <c r="J55" s="1">
         <v>5</v>
@@ -4579,8 +5368,8 @@
       <c r="H56" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I56" s="1">
-        <v>50019</v>
+      <c r="I56" s="2" t="s">
+        <v>581</v>
       </c>
       <c r="J56" s="1">
         <v>5</v>
@@ -4617,8 +5406,8 @@
       <c r="H57" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I57" s="1">
-        <v>50020</v>
+      <c r="I57" s="2" t="s">
+        <v>582</v>
       </c>
       <c r="J57" s="1">
         <v>5</v>
@@ -4655,8 +5444,8 @@
       <c r="H58" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I58" s="1">
-        <v>70001</v>
+      <c r="I58" s="2" t="s">
+        <v>583</v>
       </c>
       <c r="J58" s="1">
         <v>7</v>
@@ -4693,8 +5482,8 @@
       <c r="H59" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I59" s="1">
-        <v>70002</v>
+      <c r="I59" s="2" t="s">
+        <v>584</v>
       </c>
       <c r="J59" s="1">
         <v>7</v>
@@ -4731,8 +5520,8 @@
       <c r="H60" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I60" s="1">
-        <v>70003</v>
+      <c r="I60" s="2" t="s">
+        <v>585</v>
       </c>
       <c r="J60" s="1">
         <v>7</v>
@@ -4769,8 +5558,8 @@
       <c r="H61" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="I61" s="1">
-        <v>70004</v>
+      <c r="I61" s="2" t="s">
+        <v>586</v>
       </c>
       <c r="J61" s="1">
         <v>7</v>
@@ -4807,8 +5596,8 @@
       <c r="H62" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="I62" s="1">
-        <v>70005</v>
+      <c r="I62" s="2" t="s">
+        <v>587</v>
       </c>
       <c r="J62" s="1">
         <v>7</v>
@@ -4845,8 +5634,8 @@
       <c r="H63" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I63" s="1">
-        <v>70006</v>
+      <c r="I63" s="2" t="s">
+        <v>588</v>
       </c>
       <c r="J63" s="1">
         <v>7</v>
@@ -4883,8 +5672,8 @@
       <c r="H64" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I64" s="1">
-        <v>70007</v>
+      <c r="I64" s="2" t="s">
+        <v>589</v>
       </c>
       <c r="J64" s="1">
         <v>7</v>
@@ -4921,8 +5710,8 @@
       <c r="H65" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="I65" s="1">
-        <v>70008</v>
+      <c r="I65" s="2" t="s">
+        <v>590</v>
       </c>
       <c r="J65" s="1">
         <v>7</v>
@@ -4959,8 +5748,8 @@
       <c r="H66" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="I66" s="1">
-        <v>70009</v>
+      <c r="I66" s="2" t="s">
+        <v>591</v>
       </c>
       <c r="J66" s="1">
         <v>7</v>
@@ -4997,8 +5786,8 @@
       <c r="H67" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I67" s="1">
-        <v>70010</v>
+      <c r="I67" s="2" t="s">
+        <v>592</v>
       </c>
       <c r="J67" s="1">
         <v>7</v>
@@ -5035,8 +5824,8 @@
       <c r="H68" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="I68" s="1">
-        <v>70011</v>
+      <c r="I68" s="2" t="s">
+        <v>593</v>
       </c>
       <c r="J68" s="1">
         <v>7</v>
@@ -5073,8 +5862,8 @@
       <c r="H69" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="I69" s="1">
-        <v>70012</v>
+      <c r="I69" s="2" t="s">
+        <v>594</v>
       </c>
       <c r="J69" s="1">
         <v>7</v>
@@ -5111,8 +5900,8 @@
       <c r="H70" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="I70" s="1">
-        <v>70013</v>
+      <c r="I70" s="2" t="s">
+        <v>595</v>
       </c>
       <c r="J70" s="1">
         <v>7</v>
@@ -5149,8 +5938,8 @@
       <c r="H71" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I71" s="1">
-        <v>70014</v>
+      <c r="I71" s="2" t="s">
+        <v>596</v>
       </c>
       <c r="J71" s="1">
         <v>7</v>
@@ -5187,8 +5976,8 @@
       <c r="H72" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="I72" s="1">
-        <v>70015</v>
+      <c r="I72" s="2" t="s">
+        <v>597</v>
       </c>
       <c r="J72" s="1">
         <v>7</v>
@@ -5225,8 +6014,8 @@
       <c r="H73" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I73" s="1">
-        <v>70016</v>
+      <c r="I73" s="2" t="s">
+        <v>598</v>
       </c>
       <c r="J73" s="1">
         <v>7</v>
@@ -5263,8 +6052,8 @@
       <c r="H74" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="I74" s="1">
-        <v>70017</v>
+      <c r="I74" s="2" t="s">
+        <v>599</v>
       </c>
       <c r="J74" s="1">
         <v>7</v>
@@ -5301,8 +6090,8 @@
       <c r="H75" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I75" s="1">
-        <v>70018</v>
+      <c r="I75" s="2" t="s">
+        <v>600</v>
       </c>
       <c r="J75" s="1">
         <v>7</v>
@@ -5339,8 +6128,8 @@
       <c r="H76" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="I76" s="1">
-        <v>70019</v>
+      <c r="I76" s="2" t="s">
+        <v>601</v>
       </c>
       <c r="J76" s="1">
         <v>7</v>
@@ -5377,8 +6166,8 @@
       <c r="H77" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="I77" s="1">
-        <v>70020</v>
+      <c r="I77" s="2" t="s">
+        <v>602</v>
       </c>
       <c r="J77" s="1">
         <v>7</v>
@@ -5415,8 +6204,8 @@
       <c r="H78" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="I78" s="1">
-        <v>70021</v>
+      <c r="I78" s="2" t="s">
+        <v>603</v>
       </c>
       <c r="J78" s="1">
         <v>7</v>
@@ -5453,8 +6242,8 @@
       <c r="H79" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I79" s="1">
-        <v>70022</v>
+      <c r="I79" s="2" t="s">
+        <v>604</v>
       </c>
       <c r="J79" s="1">
         <v>7</v>
@@ -5491,8 +6280,8 @@
       <c r="H80" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="I80" s="1">
-        <v>70023</v>
+      <c r="I80" s="2" t="s">
+        <v>605</v>
       </c>
       <c r="J80" s="1">
         <v>7</v>
@@ -5529,8 +6318,8 @@
       <c r="H81" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I81" s="1">
-        <v>70024</v>
+      <c r="I81" s="2" t="s">
+        <v>606</v>
       </c>
       <c r="J81" s="1">
         <v>7</v>
@@ -5567,8 +6356,8 @@
       <c r="H82" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="I82" s="1">
-        <v>70025</v>
+      <c r="I82" s="2" t="s">
+        <v>607</v>
       </c>
       <c r="J82" s="1">
         <v>7</v>
@@ -5605,8 +6394,8 @@
       <c r="H83" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I83" s="1">
-        <v>70026</v>
+      <c r="I83" s="2" t="s">
+        <v>608</v>
       </c>
       <c r="J83" s="1">
         <v>7</v>
@@ -5643,8 +6432,8 @@
       <c r="H84" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="I84" s="1">
-        <v>70027</v>
+      <c r="I84" s="2" t="s">
+        <v>609</v>
       </c>
       <c r="J84" s="1">
         <v>7</v>
@@ -5681,8 +6470,8 @@
       <c r="H85" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="I85" s="1">
-        <v>70028</v>
+      <c r="I85" s="2" t="s">
+        <v>610</v>
       </c>
       <c r="J85" s="1">
         <v>7</v>
@@ -5719,8 +6508,8 @@
       <c r="H86" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="I86" s="1">
-        <v>70029</v>
+      <c r="I86" s="2" t="s">
+        <v>611</v>
       </c>
       <c r="J86" s="1">
         <v>7</v>
@@ -5757,8 +6546,8 @@
       <c r="H87" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I87" s="1">
-        <v>70030</v>
+      <c r="I87" s="2" t="s">
+        <v>612</v>
       </c>
       <c r="J87" s="1">
         <v>7</v>
@@ -5795,8 +6584,8 @@
       <c r="H88" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="I88" s="1">
-        <v>70031</v>
+      <c r="I88" s="2" t="s">
+        <v>613</v>
       </c>
       <c r="J88" s="1">
         <v>7</v>
@@ -5833,8 +6622,8 @@
       <c r="H89" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I89" s="1">
-        <v>70032</v>
+      <c r="I89" s="2" t="s">
+        <v>614</v>
       </c>
       <c r="J89" s="1">
         <v>7</v>
@@ -5871,8 +6660,8 @@
       <c r="H90" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="I90" s="1">
-        <v>70033</v>
+      <c r="I90" s="2" t="s">
+        <v>615</v>
       </c>
       <c r="J90" s="1">
         <v>7</v>
@@ -5909,8 +6698,8 @@
       <c r="H91" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I91" s="1">
-        <v>70034</v>
+      <c r="I91" s="2" t="s">
+        <v>616</v>
       </c>
       <c r="J91" s="1">
         <v>7</v>
@@ -5947,8 +6736,8 @@
       <c r="H92" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I92" s="1">
-        <v>70035</v>
+      <c r="I92" s="2" t="s">
+        <v>617</v>
       </c>
       <c r="J92" s="1">
         <v>7</v>
@@ -5985,8 +6774,8 @@
       <c r="H93" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="I93" s="1">
-        <v>70036</v>
+      <c r="I93" s="2" t="s">
+        <v>618</v>
       </c>
       <c r="J93" s="1">
         <v>7</v>
@@ -6023,8 +6812,8 @@
       <c r="H94" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="I94" s="1">
-        <v>70037</v>
+      <c r="I94" s="2" t="s">
+        <v>619</v>
       </c>
       <c r="J94" s="1">
         <v>7</v>
@@ -6061,8 +6850,8 @@
       <c r="H95" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="I95" s="1">
-        <v>70038</v>
+      <c r="I95" s="2" t="s">
+        <v>620</v>
       </c>
       <c r="J95" s="1">
         <v>7</v>
@@ -6099,8 +6888,8 @@
       <c r="H96" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="I96" s="1">
-        <v>70039</v>
+      <c r="I96" s="2" t="s">
+        <v>621</v>
       </c>
       <c r="J96" s="1">
         <v>7</v>
@@ -6137,8 +6926,8 @@
       <c r="H97" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="I97" s="1">
-        <v>70040</v>
+      <c r="I97" s="2" t="s">
+        <v>622</v>
       </c>
       <c r="J97" s="1">
         <v>7</v>
@@ -6175,8 +6964,8 @@
       <c r="H98" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="I98" s="1">
-        <v>70041</v>
+      <c r="I98" s="2" t="s">
+        <v>623</v>
       </c>
       <c r="J98" s="1">
         <v>7</v>
@@ -6213,8 +7002,8 @@
       <c r="H99" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I99" s="1">
-        <v>70042</v>
+      <c r="I99" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="J99" s="1">
         <v>7</v>
@@ -6251,8 +7040,8 @@
       <c r="H100" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="I100" s="1">
-        <v>70043</v>
+      <c r="I100" s="2" t="s">
+        <v>625</v>
       </c>
       <c r="J100" s="1">
         <v>7</v>
@@ -6289,8 +7078,8 @@
       <c r="H101" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I101" s="1">
-        <v>70044</v>
+      <c r="I101" s="2" t="s">
+        <v>626</v>
       </c>
       <c r="J101" s="1">
         <v>7</v>
@@ -6327,8 +7116,8 @@
       <c r="H102" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="I102" s="1">
-        <v>70045</v>
+      <c r="I102" s="2" t="s">
+        <v>627</v>
       </c>
       <c r="J102" s="1">
         <v>7</v>
@@ -6365,8 +7154,8 @@
       <c r="H103" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I103" s="1">
-        <v>70046</v>
+      <c r="I103" s="2" t="s">
+        <v>628</v>
       </c>
       <c r="J103" s="1">
         <v>7</v>
@@ -6403,8 +7192,8 @@
       <c r="H104" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="I104" s="1">
-        <v>70047</v>
+      <c r="I104" s="2" t="s">
+        <v>629</v>
       </c>
       <c r="J104" s="1">
         <v>7</v>
@@ -6441,8 +7230,8 @@
       <c r="H105" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="I105" s="1">
-        <v>70048</v>
+      <c r="I105" s="2" t="s">
+        <v>630</v>
       </c>
       <c r="J105" s="1">
         <v>7</v>
@@ -6479,8 +7268,8 @@
       <c r="H106" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="I106" s="1">
-        <v>70049</v>
+      <c r="I106" s="2" t="s">
+        <v>631</v>
       </c>
       <c r="J106" s="1">
         <v>7</v>
@@ -6517,8 +7306,8 @@
       <c r="H107" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="I107" s="1">
-        <v>70050</v>
+      <c r="I107" s="2" t="s">
+        <v>632</v>
       </c>
       <c r="J107" s="1">
         <v>7</v>
@@ -6555,8 +7344,8 @@
       <c r="H108" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I108" s="1">
-        <v>70051</v>
+      <c r="I108" s="2" t="s">
+        <v>633</v>
       </c>
       <c r="J108" s="1">
         <v>7</v>
@@ -6593,8 +7382,8 @@
       <c r="H109" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="I109" s="1">
-        <v>60001</v>
+      <c r="I109" s="2" t="s">
+        <v>634</v>
       </c>
       <c r="J109" s="1">
         <v>6</v>
@@ -6631,8 +7420,8 @@
       <c r="H110" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I110" s="1">
-        <v>60002</v>
+      <c r="I110" s="2" t="s">
+        <v>635</v>
       </c>
       <c r="J110" s="1">
         <v>6</v>
@@ -6669,8 +7458,8 @@
       <c r="H111" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="I111" s="1">
-        <v>60003</v>
+      <c r="I111" s="2" t="s">
+        <v>636</v>
       </c>
       <c r="J111" s="1">
         <v>6</v>
@@ -6707,8 +7496,8 @@
       <c r="H112" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="I112" s="1">
-        <v>60004</v>
+      <c r="I112" s="2" t="s">
+        <v>637</v>
       </c>
       <c r="J112" s="1">
         <v>6</v>
@@ -6745,8 +7534,8 @@
       <c r="H113" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I113" s="1">
-        <v>60005</v>
+      <c r="I113" s="2" t="s">
+        <v>638</v>
       </c>
       <c r="J113" s="1">
         <v>6</v>
@@ -6783,8 +7572,8 @@
       <c r="H114" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I114" s="1">
-        <v>60006</v>
+      <c r="I114" s="2" t="s">
+        <v>639</v>
       </c>
       <c r="J114" s="1">
         <v>6</v>
@@ -6821,8 +7610,8 @@
       <c r="H115" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I115" s="1">
-        <v>60007</v>
+      <c r="I115" s="2" t="s">
+        <v>640</v>
       </c>
       <c r="J115" s="1">
         <v>6</v>
@@ -6859,8 +7648,8 @@
       <c r="H116" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="I116" s="1">
-        <v>60008</v>
+      <c r="I116" s="2" t="s">
+        <v>641</v>
       </c>
       <c r="J116" s="1">
         <v>6</v>
@@ -6897,8 +7686,8 @@
       <c r="H117" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="I117" s="1">
-        <v>60009</v>
+      <c r="I117" s="2" t="s">
+        <v>642</v>
       </c>
       <c r="J117" s="1">
         <v>6</v>
@@ -6935,8 +7724,8 @@
       <c r="H118" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="I118" s="1">
-        <v>60010</v>
+      <c r="I118" s="2" t="s">
+        <v>643</v>
       </c>
       <c r="J118" s="1">
         <v>6</v>
@@ -6973,8 +7762,8 @@
       <c r="H119" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="I119" s="1">
-        <v>60011</v>
+      <c r="I119" s="2" t="s">
+        <v>644</v>
       </c>
       <c r="J119" s="1">
         <v>6</v>
@@ -7011,8 +7800,8 @@
       <c r="H120" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="I120" s="1">
-        <v>60012</v>
+      <c r="I120" s="2" t="s">
+        <v>645</v>
       </c>
       <c r="J120" s="1">
         <v>6</v>
@@ -7049,8 +7838,8 @@
       <c r="H121" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I121" s="1">
-        <v>60013</v>
+      <c r="I121" s="2" t="s">
+        <v>646</v>
       </c>
       <c r="J121" s="1">
         <v>6</v>
@@ -7087,8 +7876,8 @@
       <c r="H122" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I122" s="1">
-        <v>60014</v>
+      <c r="I122" s="2" t="s">
+        <v>647</v>
       </c>
       <c r="J122" s="1">
         <v>6</v>
@@ -7125,8 +7914,8 @@
       <c r="H123" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="I123" s="1">
-        <v>60015</v>
+      <c r="I123" s="2" t="s">
+        <v>648</v>
       </c>
       <c r="J123" s="1">
         <v>6</v>
@@ -7163,8 +7952,8 @@
       <c r="H124" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="I124" s="1">
-        <v>60016</v>
+      <c r="I124" s="2" t="s">
+        <v>649</v>
       </c>
       <c r="J124" s="1">
         <v>6</v>
@@ -7201,8 +7990,8 @@
       <c r="H125" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I125" s="1">
-        <v>60017</v>
+      <c r="I125" s="2" t="s">
+        <v>650</v>
       </c>
       <c r="J125" s="1">
         <v>6</v>
@@ -7239,8 +8028,8 @@
       <c r="H126" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I126" s="1">
-        <v>60018</v>
+      <c r="I126" s="2" t="s">
+        <v>651</v>
       </c>
       <c r="J126" s="1">
         <v>6</v>
@@ -7277,8 +8066,8 @@
       <c r="H127" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I127" s="1">
-        <v>60019</v>
+      <c r="I127" s="2" t="s">
+        <v>652</v>
       </c>
       <c r="J127" s="1">
         <v>6</v>
@@ -7315,8 +8104,8 @@
       <c r="H128" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="I128" s="1">
-        <v>60020</v>
+      <c r="I128" s="2" t="s">
+        <v>653</v>
       </c>
       <c r="J128" s="1">
         <v>6</v>
@@ -7353,8 +8142,8 @@
       <c r="H129" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="I129" s="1">
-        <v>60021</v>
+      <c r="I129" s="2" t="s">
+        <v>654</v>
       </c>
       <c r="J129" s="1">
         <v>6</v>
@@ -7391,8 +8180,8 @@
       <c r="H130" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="I130" s="1">
-        <v>60022</v>
+      <c r="I130" s="2" t="s">
+        <v>655</v>
       </c>
       <c r="J130" s="1">
         <v>6</v>
@@ -7429,8 +8218,8 @@
       <c r="H131" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="I131" s="1">
-        <v>60023</v>
+      <c r="I131" s="2" t="s">
+        <v>656</v>
       </c>
       <c r="J131" s="1">
         <v>6</v>
@@ -7467,8 +8256,8 @@
       <c r="H132" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I132" s="1">
-        <v>60024</v>
+      <c r="I132" s="2" t="s">
+        <v>657</v>
       </c>
       <c r="J132" s="1">
         <v>6</v>
@@ -7505,8 +8294,8 @@
       <c r="H133" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="I133" s="1">
-        <v>60025</v>
+      <c r="I133" s="2" t="s">
+        <v>658</v>
       </c>
       <c r="J133" s="1">
         <v>6</v>
@@ -7543,8 +8332,8 @@
       <c r="H134" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="I134" s="1">
-        <v>60026</v>
+      <c r="I134" s="2" t="s">
+        <v>659</v>
       </c>
       <c r="J134" s="1">
         <v>6</v>
@@ -7581,8 +8370,8 @@
       <c r="H135" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="I135" s="1">
-        <v>60027</v>
+      <c r="I135" s="2" t="s">
+        <v>660</v>
       </c>
       <c r="J135" s="1">
         <v>6</v>
@@ -7619,8 +8408,8 @@
       <c r="H136" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I136" s="1">
-        <v>60028</v>
+      <c r="I136" s="2" t="s">
+        <v>661</v>
       </c>
       <c r="J136" s="1">
         <v>6</v>
@@ -7657,8 +8446,8 @@
       <c r="H137" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="I137" s="1">
-        <v>60029</v>
+      <c r="I137" s="2" t="s">
+        <v>662</v>
       </c>
       <c r="J137" s="1">
         <v>6</v>
@@ -7695,8 +8484,8 @@
       <c r="H138" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I138" s="1">
-        <v>60030</v>
+      <c r="I138" s="2" t="s">
+        <v>663</v>
       </c>
       <c r="J138" s="1">
         <v>6</v>
@@ -7733,8 +8522,8 @@
       <c r="H139" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I139" s="1">
-        <v>60031</v>
+      <c r="I139" s="2" t="s">
+        <v>664</v>
       </c>
       <c r="J139" s="1">
         <v>6</v>
@@ -7771,8 +8560,8 @@
       <c r="H140" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I140" s="1">
-        <v>60032</v>
+      <c r="I140" s="2" t="s">
+        <v>665</v>
       </c>
       <c r="J140" s="1">
         <v>6</v>
@@ -7809,8 +8598,8 @@
       <c r="H141" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="I141" s="1">
-        <v>60033</v>
+      <c r="I141" s="2" t="s">
+        <v>666</v>
       </c>
       <c r="J141" s="1">
         <v>6</v>
@@ -7847,8 +8636,8 @@
       <c r="H142" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I142" s="1">
-        <v>60034</v>
+      <c r="I142" s="2" t="s">
+        <v>667</v>
       </c>
       <c r="J142" s="1">
         <v>6</v>
@@ -7885,8 +8674,8 @@
       <c r="H143" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="I143" s="1">
-        <v>60035</v>
+      <c r="I143" s="2" t="s">
+        <v>668</v>
       </c>
       <c r="J143" s="1">
         <v>6</v>
@@ -7923,8 +8712,8 @@
       <c r="H144" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="I144" s="1">
-        <v>60036</v>
+      <c r="I144" s="2" t="s">
+        <v>669</v>
       </c>
       <c r="J144" s="1">
         <v>6</v>
@@ -7961,8 +8750,8 @@
       <c r="H145" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="I145" s="1">
-        <v>60037</v>
+      <c r="I145" s="2" t="s">
+        <v>670</v>
       </c>
       <c r="J145" s="1">
         <v>6</v>
@@ -7999,8 +8788,8 @@
       <c r="H146" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="I146" s="1">
-        <v>60038</v>
+      <c r="I146" s="2" t="s">
+        <v>671</v>
       </c>
       <c r="J146" s="1">
         <v>6</v>
@@ -8037,8 +8826,8 @@
       <c r="H147" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="I147" s="1">
-        <v>60039</v>
+      <c r="I147" s="2" t="s">
+        <v>672</v>
       </c>
       <c r="J147" s="1">
         <v>6</v>
@@ -8075,8 +8864,8 @@
       <c r="H148" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="I148" s="1">
-        <v>60040</v>
+      <c r="I148" s="2" t="s">
+        <v>673</v>
       </c>
       <c r="J148" s="1">
         <v>6</v>
@@ -8113,8 +8902,8 @@
       <c r="H149" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="I149" s="1">
-        <v>60041</v>
+      <c r="I149" s="2" t="s">
+        <v>674</v>
       </c>
       <c r="J149" s="1">
         <v>6</v>
@@ -8151,8 +8940,8 @@
       <c r="H150" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I150" s="1">
-        <v>60042</v>
+      <c r="I150" s="2" t="s">
+        <v>675</v>
       </c>
       <c r="J150" s="1">
         <v>6</v>
@@ -8189,8 +8978,8 @@
       <c r="H151" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="I151" s="1">
-        <v>60043</v>
+      <c r="I151" s="2" t="s">
+        <v>676</v>
       </c>
       <c r="J151" s="1">
         <v>6</v>
@@ -8227,8 +9016,8 @@
       <c r="H152" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="I152" s="1">
-        <v>60044</v>
+      <c r="I152" s="2" t="s">
+        <v>677</v>
       </c>
       <c r="J152" s="1">
         <v>6</v>
@@ -8265,8 +9054,8 @@
       <c r="H153" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I153" s="1">
-        <v>60045</v>
+      <c r="I153" s="2" t="s">
+        <v>678</v>
       </c>
       <c r="J153" s="1">
         <v>6</v>
@@ -8303,8 +9092,8 @@
       <c r="H154" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I154" s="1">
-        <v>60046</v>
+      <c r="I154" s="2" t="s">
+        <v>679</v>
       </c>
       <c r="J154" s="1">
         <v>6</v>
@@ -8341,8 +9130,8 @@
       <c r="H155" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I155" s="1">
-        <v>60047</v>
+      <c r="I155" s="2" t="s">
+        <v>680</v>
       </c>
       <c r="J155" s="1">
         <v>6</v>
@@ -8379,8 +9168,8 @@
       <c r="H156" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="I156" s="1">
-        <v>60048</v>
+      <c r="I156" s="2" t="s">
+        <v>681</v>
       </c>
       <c r="J156" s="1">
         <v>6</v>
@@ -8417,8 +9206,8 @@
       <c r="H157" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I157" s="1">
-        <v>60049</v>
+      <c r="I157" s="2" t="s">
+        <v>682</v>
       </c>
       <c r="J157" s="1">
         <v>6</v>
@@ -8455,8 +9244,8 @@
       <c r="H158" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="I158" s="1">
-        <v>60050</v>
+      <c r="I158" s="2" t="s">
+        <v>683</v>
       </c>
       <c r="J158" s="1">
         <v>6</v>
@@ -8493,8 +9282,8 @@
       <c r="H159" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I159" s="1">
-        <v>60051</v>
+      <c r="I159" s="2" t="s">
+        <v>684</v>
       </c>
       <c r="J159" s="1">
         <v>6</v>
@@ -8531,8 +9320,8 @@
       <c r="H160" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="I160" s="1">
-        <v>60052</v>
+      <c r="I160" s="2" t="s">
+        <v>685</v>
       </c>
       <c r="J160" s="1">
         <v>6</v>
@@ -8569,8 +9358,8 @@
       <c r="H161" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I161" s="1">
-        <v>60053</v>
+      <c r="I161" s="2" t="s">
+        <v>686</v>
       </c>
       <c r="J161" s="1">
         <v>6</v>
@@ -8607,8 +9396,8 @@
       <c r="H162" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I162" s="1">
-        <v>60054</v>
+      <c r="I162" s="2" t="s">
+        <v>687</v>
       </c>
       <c r="J162" s="1">
         <v>6</v>
@@ -8645,8 +9434,8 @@
       <c r="H163" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="I163" s="1">
-        <v>60055</v>
+      <c r="I163" s="2" t="s">
+        <v>688</v>
       </c>
       <c r="J163" s="1">
         <v>6</v>
@@ -8683,8 +9472,8 @@
       <c r="H164" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I164" s="1">
-        <v>60056</v>
+      <c r="I164" s="2" t="s">
+        <v>689</v>
       </c>
       <c r="J164" s="1">
         <v>6</v>
@@ -8721,8 +9510,8 @@
       <c r="H165" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="I165" s="1">
-        <v>60057</v>
+      <c r="I165" s="2" t="s">
+        <v>690</v>
       </c>
       <c r="J165" s="1">
         <v>6</v>
@@ -8759,8 +9548,8 @@
       <c r="H166" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="I166" s="1">
-        <v>60058</v>
+      <c r="I166" s="2" t="s">
+        <v>691</v>
       </c>
       <c r="J166" s="1">
         <v>6</v>
@@ -8797,8 +9586,8 @@
       <c r="H167" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="I167" s="1">
-        <v>60059</v>
+      <c r="I167" s="2" t="s">
+        <v>692</v>
       </c>
       <c r="J167" s="1">
         <v>6</v>
@@ -8835,8 +9624,8 @@
       <c r="H168" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="I168" s="1">
-        <v>60060</v>
+      <c r="I168" s="2" t="s">
+        <v>693</v>
       </c>
       <c r="J168" s="1">
         <v>6</v>
@@ -8873,8 +9662,8 @@
       <c r="H169" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I169" s="1">
-        <v>60061</v>
+      <c r="I169" s="2" t="s">
+        <v>694</v>
       </c>
       <c r="J169" s="1">
         <v>6</v>
@@ -8911,8 +9700,8 @@
       <c r="H170" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="I170" s="1">
-        <v>60062</v>
+      <c r="I170" s="2" t="s">
+        <v>695</v>
       </c>
       <c r="J170" s="1">
         <v>6</v>
@@ -8949,8 +9738,8 @@
       <c r="H171" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I171" s="1">
-        <v>60063</v>
+      <c r="I171" s="2" t="s">
+        <v>696</v>
       </c>
       <c r="J171" s="1">
         <v>6</v>
@@ -8987,8 +9776,8 @@
       <c r="H172" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="I172" s="1">
-        <v>60064</v>
+      <c r="I172" s="2" t="s">
+        <v>697</v>
       </c>
       <c r="J172" s="1">
         <v>6</v>
@@ -9025,8 +9814,8 @@
       <c r="H173" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="I173" s="1">
-        <v>60065</v>
+      <c r="I173" s="2" t="s">
+        <v>698</v>
       </c>
       <c r="J173" s="1">
         <v>6</v>
@@ -9063,8 +9852,8 @@
       <c r="H174" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="I174" s="1">
-        <v>60066</v>
+      <c r="I174" s="2" t="s">
+        <v>699</v>
       </c>
       <c r="J174" s="1">
         <v>6</v>
@@ -9101,8 +9890,8 @@
       <c r="H175" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I175" s="1">
-        <v>60067</v>
+      <c r="I175" s="2" t="s">
+        <v>700</v>
       </c>
       <c r="J175" s="1">
         <v>6</v>
@@ -9139,8 +9928,8 @@
       <c r="H176" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="I176" s="1">
-        <v>60068</v>
+      <c r="I176" s="2" t="s">
+        <v>701</v>
       </c>
       <c r="J176" s="1">
         <v>6</v>
@@ -9177,8 +9966,8 @@
       <c r="H177" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="I177" s="1">
-        <v>60069</v>
+      <c r="I177" s="2" t="s">
+        <v>702</v>
       </c>
       <c r="J177" s="1">
         <v>6</v>
@@ -9215,8 +10004,8 @@
       <c r="H178" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="I178" s="1">
-        <v>60070</v>
+      <c r="I178" s="2" t="s">
+        <v>703</v>
       </c>
       <c r="J178" s="1">
         <v>6</v>
@@ -9253,8 +10042,8 @@
       <c r="H179" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I179" s="1">
-        <v>60071</v>
+      <c r="I179" s="2" t="s">
+        <v>704</v>
       </c>
       <c r="J179" s="1">
         <v>6</v>
@@ -9291,8 +10080,8 @@
       <c r="H180" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="I180" s="1">
-        <v>60072</v>
+      <c r="I180" s="2" t="s">
+        <v>705</v>
       </c>
       <c r="J180" s="1">
         <v>6</v>
@@ -9329,8 +10118,8 @@
       <c r="H181" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="I181" s="1">
-        <v>60073</v>
+      <c r="I181" s="2" t="s">
+        <v>706</v>
       </c>
       <c r="J181" s="1">
         <v>6</v>
@@ -9367,8 +10156,8 @@
       <c r="H182" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="I182" s="1">
-        <v>60074</v>
+      <c r="I182" s="2" t="s">
+        <v>707</v>
       </c>
       <c r="J182" s="1">
         <v>6</v>
@@ -9405,8 +10194,8 @@
       <c r="H183" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="I183" s="1">
-        <v>60075</v>
+      <c r="I183" s="2" t="s">
+        <v>708</v>
       </c>
       <c r="J183" s="1">
         <v>6</v>
@@ -9443,8 +10232,8 @@
       <c r="H184" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="I184" s="1">
-        <v>60076</v>
+      <c r="I184" s="2" t="s">
+        <v>709</v>
       </c>
       <c r="J184" s="1">
         <v>6</v>
@@ -9481,8 +10270,8 @@
       <c r="H185" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="I185" s="1">
-        <v>60077</v>
+      <c r="I185" s="2" t="s">
+        <v>710</v>
       </c>
       <c r="J185" s="1">
         <v>6</v>
@@ -9519,8 +10308,8 @@
       <c r="H186" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I186" s="1">
-        <v>60078</v>
+      <c r="I186" s="2" t="s">
+        <v>711</v>
       </c>
       <c r="J186" s="1">
         <v>6</v>
@@ -9557,8 +10346,8 @@
       <c r="H187" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="I187" s="1">
-        <v>60079</v>
+      <c r="I187" s="2" t="s">
+        <v>712</v>
       </c>
       <c r="J187" s="1">
         <v>6</v>
@@ -9595,8 +10384,8 @@
       <c r="H188" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="I188" s="1">
-        <v>60080</v>
+      <c r="I188" s="2" t="s">
+        <v>713</v>
       </c>
       <c r="J188" s="1">
         <v>6</v>
@@ -9633,8 +10422,8 @@
       <c r="H189" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="I189" s="1">
-        <v>60081</v>
+      <c r="I189" s="2" t="s">
+        <v>714</v>
       </c>
       <c r="J189" s="1">
         <v>6</v>
@@ -9671,8 +10460,8 @@
       <c r="H190" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="I190" s="1">
-        <v>60082</v>
+      <c r="I190" s="2" t="s">
+        <v>715</v>
       </c>
       <c r="J190" s="1">
         <v>6</v>
@@ -9709,8 +10498,8 @@
       <c r="H191" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="I191" s="1">
-        <v>60083</v>
+      <c r="I191" s="2" t="s">
+        <v>716</v>
       </c>
       <c r="J191" s="1">
         <v>6</v>
@@ -9747,8 +10536,8 @@
       <c r="H192" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="I192" s="1">
-        <v>60084</v>
+      <c r="I192" s="2" t="s">
+        <v>717</v>
       </c>
       <c r="J192" s="1">
         <v>6</v>
@@ -9785,8 +10574,8 @@
       <c r="H193" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I193" s="1">
-        <v>60085</v>
+      <c r="I193" s="2" t="s">
+        <v>718</v>
       </c>
       <c r="J193" s="1">
         <v>6</v>
@@ -9823,8 +10612,8 @@
       <c r="H194" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="I194" s="1">
-        <v>60086</v>
+      <c r="I194" s="2" t="s">
+        <v>719</v>
       </c>
       <c r="J194" s="1">
         <v>6</v>
@@ -9861,8 +10650,8 @@
       <c r="H195" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I195" s="1">
-        <v>60087</v>
+      <c r="I195" s="2" t="s">
+        <v>720</v>
       </c>
       <c r="J195" s="1">
         <v>6</v>
@@ -9899,8 +10688,8 @@
       <c r="H196" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I196" s="1">
-        <v>60088</v>
+      <c r="I196" s="2" t="s">
+        <v>721</v>
       </c>
       <c r="J196" s="1">
         <v>6</v>
@@ -9937,8 +10726,8 @@
       <c r="H197" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="I197" s="1">
-        <v>60089</v>
+      <c r="I197" s="2" t="s">
+        <v>722</v>
       </c>
       <c r="J197" s="1">
         <v>6</v>
@@ -9975,8 +10764,8 @@
       <c r="H198" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="I198" s="1">
-        <v>60090</v>
+      <c r="I198" s="2" t="s">
+        <v>723</v>
       </c>
       <c r="J198" s="1">
         <v>6</v>
@@ -10013,8 +10802,8 @@
       <c r="H199" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I199" s="1">
-        <v>60091</v>
+      <c r="I199" s="2" t="s">
+        <v>724</v>
       </c>
       <c r="J199" s="1">
         <v>6</v>
@@ -10051,8 +10840,8 @@
       <c r="H200" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="I200" s="1">
-        <v>60092</v>
+      <c r="I200" s="2" t="s">
+        <v>725</v>
       </c>
       <c r="J200" s="1">
         <v>6</v>
@@ -10089,8 +10878,8 @@
       <c r="H201" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I201" s="1">
-        <v>60093</v>
+      <c r="I201" s="2" t="s">
+        <v>726</v>
       </c>
       <c r="J201" s="1">
         <v>6</v>
@@ -10127,8 +10916,8 @@
       <c r="H202" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="I202" s="1">
-        <v>60094</v>
+      <c r="I202" s="2" t="s">
+        <v>727</v>
       </c>
       <c r="J202" s="1">
         <v>6</v>
@@ -10165,8 +10954,8 @@
       <c r="H203" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I203" s="1">
-        <v>60095</v>
+      <c r="I203" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="J203" s="1">
         <v>6</v>
@@ -10203,8 +10992,8 @@
       <c r="H204" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I204" s="1">
-        <v>60096</v>
+      <c r="I204" s="2" t="s">
+        <v>729</v>
       </c>
       <c r="J204" s="1">
         <v>6</v>
@@ -10241,8 +11030,8 @@
       <c r="H205" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I205" s="1">
-        <v>60097</v>
+      <c r="I205" s="2" t="s">
+        <v>730</v>
       </c>
       <c r="J205" s="1">
         <v>6</v>
@@ -10279,8 +11068,8 @@
       <c r="H206" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="I206" s="1">
-        <v>80001</v>
+      <c r="I206" s="2" t="s">
+        <v>731</v>
       </c>
       <c r="J206" s="1">
         <v>8</v>
@@ -10317,8 +11106,8 @@
       <c r="H207" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I207" s="1">
-        <v>80002</v>
+      <c r="I207" s="2" t="s">
+        <v>732</v>
       </c>
       <c r="J207" s="1">
         <v>8</v>
@@ -10355,8 +11144,8 @@
       <c r="H208" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I208" s="1">
-        <v>80003</v>
+      <c r="I208" s="2" t="s">
+        <v>733</v>
       </c>
       <c r="J208" s="1">
         <v>8</v>
@@ -10393,8 +11182,8 @@
       <c r="H209" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I209" s="1">
-        <v>80004</v>
+      <c r="I209" s="2" t="s">
+        <v>734</v>
       </c>
       <c r="J209" s="1">
         <v>8</v>
@@ -10431,8 +11220,8 @@
       <c r="H210" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="I210" s="1">
-        <v>80005</v>
+      <c r="I210" s="2" t="s">
+        <v>735</v>
       </c>
       <c r="J210" s="1">
         <v>8</v>
@@ -10469,8 +11258,8 @@
       <c r="H211" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I211" s="1">
-        <v>80006</v>
+      <c r="I211" s="2" t="s">
+        <v>736</v>
       </c>
       <c r="J211" s="1">
         <v>8</v>
@@ -10507,8 +11296,8 @@
       <c r="H212" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I212" s="1">
-        <v>80007</v>
+      <c r="I212" s="2" t="s">
+        <v>737</v>
       </c>
       <c r="J212" s="1">
         <v>8</v>
@@ -10545,8 +11334,8 @@
       <c r="H213" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I213" s="1">
-        <v>80008</v>
+      <c r="I213" s="2" t="s">
+        <v>738</v>
       </c>
       <c r="J213" s="1">
         <v>8</v>
@@ -10583,8 +11372,8 @@
       <c r="H214" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I214" s="1">
-        <v>80009</v>
+      <c r="I214" s="2" t="s">
+        <v>739</v>
       </c>
       <c r="J214" s="1">
         <v>8</v>
@@ -10621,8 +11410,8 @@
       <c r="H215" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="I215" s="1">
-        <v>80010</v>
+      <c r="I215" s="2" t="s">
+        <v>740</v>
       </c>
       <c r="J215" s="1">
         <v>8</v>
@@ -10659,8 +11448,8 @@
       <c r="H216" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="I216" s="1">
-        <v>80011</v>
+      <c r="I216" s="2" t="s">
+        <v>741</v>
       </c>
       <c r="J216" s="1">
         <v>8</v>
@@ -10697,8 +11486,8 @@
       <c r="H217" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="I217" s="1">
-        <v>80012</v>
+      <c r="I217" s="2" t="s">
+        <v>742</v>
       </c>
       <c r="J217" s="1">
         <v>8</v>
@@ -10735,8 +11524,8 @@
       <c r="H218" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="I218" s="1">
-        <v>80013</v>
+      <c r="I218" s="2" t="s">
+        <v>743</v>
       </c>
       <c r="J218" s="1">
         <v>8</v>
@@ -10773,8 +11562,8 @@
       <c r="H219" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="I219" s="1">
-        <v>80014</v>
+      <c r="I219" s="2" t="s">
+        <v>744</v>
       </c>
       <c r="J219" s="1">
         <v>8</v>
@@ -10811,8 +11600,8 @@
       <c r="H220" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I220" s="1">
-        <v>80015</v>
+      <c r="I220" s="2" t="s">
+        <v>745</v>
       </c>
       <c r="J220" s="1">
         <v>8</v>
@@ -10849,8 +11638,8 @@
       <c r="H221" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I221" s="1">
-        <v>80016</v>
+      <c r="I221" s="2" t="s">
+        <v>746</v>
       </c>
       <c r="J221" s="1">
         <v>8</v>
@@ -10887,8 +11676,8 @@
       <c r="H222" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I222" s="1">
-        <v>80017</v>
+      <c r="I222" s="2" t="s">
+        <v>747</v>
       </c>
       <c r="J222" s="1">
         <v>8</v>
@@ -10925,8 +11714,8 @@
       <c r="H223" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I223" s="1">
-        <v>80018</v>
+      <c r="I223" s="2" t="s">
+        <v>748</v>
       </c>
       <c r="J223" s="1">
         <v>8</v>
@@ -10963,8 +11752,8 @@
       <c r="H224" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="I224" s="1">
-        <v>80019</v>
+      <c r="I224" s="2" t="s">
+        <v>749</v>
       </c>
       <c r="J224" s="1">
         <v>8</v>
@@ -11001,8 +11790,8 @@
       <c r="H225" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="I225" s="1">
-        <v>80020</v>
+      <c r="I225" s="2" t="s">
+        <v>750</v>
       </c>
       <c r="J225" s="1">
         <v>8</v>
@@ -11039,8 +11828,8 @@
       <c r="H226" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="I226" s="1">
-        <v>80021</v>
+      <c r="I226" s="2" t="s">
+        <v>751</v>
       </c>
       <c r="J226" s="1">
         <v>8</v>
@@ -11077,8 +11866,8 @@
       <c r="H227" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="I227" s="1">
-        <v>80022</v>
+      <c r="I227" s="2" t="s">
+        <v>752</v>
       </c>
       <c r="J227" s="1">
         <v>8</v>
@@ -11115,8 +11904,8 @@
       <c r="H228" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="I228" s="1">
-        <v>80023</v>
+      <c r="I228" s="2" t="s">
+        <v>753</v>
       </c>
       <c r="J228" s="1">
         <v>8</v>
@@ -11153,8 +11942,8 @@
       <c r="H229" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="I229" s="1">
-        <v>80024</v>
+      <c r="I229" s="2" t="s">
+        <v>754</v>
       </c>
       <c r="J229" s="1">
         <v>8</v>
@@ -11191,8 +11980,8 @@
       <c r="H230" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I230" s="1">
-        <v>80025</v>
+      <c r="I230" s="2" t="s">
+        <v>755</v>
       </c>
       <c r="J230" s="1">
         <v>8</v>
@@ -11229,8 +12018,8 @@
       <c r="H231" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="I231" s="1">
-        <v>80026</v>
+      <c r="I231" s="2" t="s">
+        <v>756</v>
       </c>
       <c r="J231" s="1">
         <v>8</v>
@@ -11267,8 +12056,8 @@
       <c r="H232" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="I232" s="1">
-        <v>110124</v>
+      <c r="I232" s="2" t="s">
+        <v>763</v>
       </c>
       <c r="J232" s="1">
         <v>11</v>
@@ -11305,8 +12094,8 @@
       <c r="H233" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="I233" s="1">
-        <v>110125</v>
+      <c r="I233" s="2" t="s">
+        <v>764</v>
       </c>
       <c r="J233" s="1">
         <v>11</v>
@@ -11343,8 +12132,8 @@
       <c r="H234" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="I234" s="1">
-        <v>110126</v>
+      <c r="I234" s="2" t="s">
+        <v>765</v>
       </c>
       <c r="J234" s="1">
         <v>11</v>
@@ -11381,8 +12170,8 @@
       <c r="H235" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I235" s="1">
-        <v>110127</v>
+      <c r="I235" s="2" t="s">
+        <v>766</v>
       </c>
       <c r="J235" s="1">
         <v>11</v>
@@ -11419,8 +12208,8 @@
       <c r="H236" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="I236" s="1">
-        <v>110128</v>
+      <c r="I236" s="2" t="s">
+        <v>767</v>
       </c>
       <c r="J236" s="1">
         <v>11</v>
@@ -11457,8 +12246,8 @@
       <c r="H237" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="I237" s="1">
-        <v>110129</v>
+      <c r="I237" s="2" t="s">
+        <v>768</v>
       </c>
       <c r="J237" s="1">
         <v>11</v>
@@ -11495,8 +12284,8 @@
       <c r="H238" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="I238" s="1">
-        <v>110130</v>
+      <c r="I238" s="2" t="s">
+        <v>769</v>
       </c>
       <c r="J238" s="1">
         <v>11</v>
@@ -11533,8 +12322,8 @@
       <c r="H239" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I239" s="1">
-        <v>110131</v>
+      <c r="I239" s="2" t="s">
+        <v>770</v>
       </c>
       <c r="J239" s="1">
         <v>11</v>
@@ -11571,8 +12360,8 @@
       <c r="H240" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="I240" s="1">
-        <v>110132</v>
+      <c r="I240" s="2" t="s">
+        <v>771</v>
       </c>
       <c r="J240" s="1">
         <v>11</v>
@@ -11609,8 +12398,8 @@
       <c r="H241" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="I241" s="1">
-        <v>110133</v>
+      <c r="I241" s="2" t="s">
+        <v>772</v>
       </c>
       <c r="J241" s="1">
         <v>11</v>
@@ -11647,8 +12436,8 @@
       <c r="H242" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="I242" s="1">
-        <v>110134</v>
+      <c r="I242" s="2" t="s">
+        <v>773</v>
       </c>
       <c r="J242" s="1">
         <v>11</v>
@@ -11685,8 +12474,8 @@
       <c r="H243" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="I243" s="1">
-        <v>110135</v>
+      <c r="I243" s="2" t="s">
+        <v>774</v>
       </c>
       <c r="J243" s="1">
         <v>11</v>
@@ -11723,8 +12512,8 @@
       <c r="H244" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="I244" s="1">
-        <v>110136</v>
+      <c r="I244" s="2" t="s">
+        <v>775</v>
       </c>
       <c r="J244" s="1">
         <v>11</v>
@@ -11761,8 +12550,8 @@
       <c r="H245" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="I245" s="1">
-        <v>110137</v>
+      <c r="I245" s="2" t="s">
+        <v>776</v>
       </c>
       <c r="J245" s="1">
         <v>11</v>
@@ -11799,8 +12588,8 @@
       <c r="H246" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I246" s="1">
-        <v>110138</v>
+      <c r="I246" s="2" t="s">
+        <v>777</v>
       </c>
       <c r="J246" s="1">
         <v>11</v>
@@ -11837,8 +12626,8 @@
       <c r="H247" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="I247" s="1">
-        <v>110139</v>
+      <c r="I247" s="2" t="s">
+        <v>778</v>
       </c>
       <c r="J247" s="1">
         <v>11</v>
@@ -11875,8 +12664,8 @@
       <c r="H248" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="I248" s="1">
-        <v>110140</v>
+      <c r="I248" s="2" t="s">
+        <v>779</v>
       </c>
       <c r="J248" s="1">
         <v>11</v>
@@ -11913,8 +12702,8 @@
       <c r="H249" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="I249" s="1">
-        <v>110141</v>
+      <c r="I249" s="2" t="s">
+        <v>780</v>
       </c>
       <c r="J249" s="1">
         <v>11</v>
@@ -11951,8 +12740,8 @@
       <c r="H250" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="I250" s="1">
-        <v>110142</v>
+      <c r="I250" s="2" t="s">
+        <v>781</v>
       </c>
       <c r="J250" s="1">
         <v>11</v>
@@ -11989,8 +12778,8 @@
       <c r="H251" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="I251" s="1">
-        <v>110143</v>
+      <c r="I251" s="2" t="s">
+        <v>782</v>
       </c>
       <c r="J251" s="1">
         <v>11</v>
@@ -12027,8 +12816,8 @@
       <c r="H252" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="I252" s="1">
-        <v>110144</v>
+      <c r="I252" s="2" t="s">
+        <v>783</v>
       </c>
       <c r="J252" s="1">
         <v>11</v>
@@ -12065,8 +12854,8 @@
       <c r="H253" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="I253" s="1">
-        <v>110145</v>
+      <c r="I253" s="2" t="s">
+        <v>784</v>
       </c>
       <c r="J253" s="1">
         <v>11</v>
@@ -12103,8 +12892,8 @@
       <c r="H254" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I254" s="1">
-        <v>110146</v>
+      <c r="I254" s="2" t="s">
+        <v>785</v>
       </c>
       <c r="J254" s="1">
         <v>11</v>
@@ -12141,8 +12930,8 @@
       <c r="H255" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I255" s="1">
-        <v>110147</v>
+      <c r="I255" s="2" t="s">
+        <v>786</v>
       </c>
       <c r="J255" s="1">
         <v>11</v>
@@ -12179,11 +12968,11 @@
       <c r="H256" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I256" s="1">
-        <v>110148</v>
+      <c r="I256" s="2" t="s">
+        <v>757</v>
       </c>
       <c r="J256" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K256" s="1" t="s">
         <v>519</v>
@@ -12217,11 +13006,11 @@
       <c r="H257" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I257" s="1">
-        <v>110149</v>
+      <c r="I257" s="2" t="s">
+        <v>758</v>
       </c>
       <c r="J257" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K257" s="1" t="s">
         <v>519</v>
@@ -12255,11 +13044,11 @@
       <c r="H258" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="I258" s="1">
-        <v>110150</v>
+      <c r="I258" s="2" t="s">
+        <v>759</v>
       </c>
       <c r="J258" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K258" s="1" t="s">
         <v>519</v>
@@ -12293,11 +13082,11 @@
       <c r="H259" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I259" s="1">
-        <v>110151</v>
+      <c r="I259" s="2" t="s">
+        <v>760</v>
       </c>
       <c r="J259" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K259" s="1" t="s">
         <v>519</v>
@@ -12331,11 +13120,11 @@
       <c r="H260" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="I260" s="1">
-        <v>110152</v>
+      <c r="I260" s="2" t="s">
+        <v>761</v>
       </c>
       <c r="J260" s="1">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="K260" s="1" t="s">
         <v>515</v>
@@ -12358,7 +13147,7 @@
         <v>11</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="F261" s="1" t="s">
         <v>516</v>
@@ -12369,17 +13158,55 @@
       <c r="H261" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="I261" s="1">
-        <v>110153</v>
+      <c r="I261" s="2" t="s">
+        <v>762</v>
       </c>
       <c r="J261" s="1">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="K261" s="1" t="s">
         <v>515</v>
       </c>
       <c r="L261" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A262" s="1">
+        <v>261</v>
+      </c>
+      <c r="B262" s="1">
+        <v>275</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F262" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="G262" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="H262" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I262" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="J262" s="1">
+        <v>23</v>
+      </c>
+      <c r="K262" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="L262" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no abrir los csv desde Excel, o ignorar como aparece el num de tarjeta
</commit_message>
<xml_diff>
--- a/Datos/personal.xlsx
+++ b/Datos/personal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605E026E-2202-4189-991B-BC098DC1DF6A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC856A5C-FAC6-421E-8780-0D0CB27203A7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3235,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="H235" sqref="H235"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="G234" sqref="G234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
habia una llave foranea mal
</commit_message>
<xml_diff>
--- a/Datos/personal.xlsx
+++ b/Datos/personal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC856A5C-FAC6-421E-8780-0D0CB27203A7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BAFF45-D19E-412A-9F35-F23216C35685}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3235,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="G234" sqref="G234"/>
+    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
+      <selection activeCell="J256" sqref="J256:J259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12972,7 +12972,7 @@
         <v>757</v>
       </c>
       <c r="J256" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="K256" s="1" t="s">
         <v>519</v>
@@ -13010,7 +13010,7 @@
         <v>758</v>
       </c>
       <c r="J257" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="K257" s="1" t="s">
         <v>519</v>
@@ -13048,7 +13048,7 @@
         <v>759</v>
       </c>
       <c r="J258" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="K258" s="1" t="s">
         <v>519</v>
@@ -13086,7 +13086,7 @@
         <v>760</v>
       </c>
       <c r="J259" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="K259" s="1" t="s">
         <v>519</v>

</xml_diff>

<commit_message>
el atributo sexo de personal esta como debe
</commit_message>
<xml_diff>
--- a/Datos/personal.xlsx
+++ b/Datos/personal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{655230A9-849B-41F6-B953-B4028BDFA4E8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B05779-BC48-4BFD-B889-E4188A992760}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="787">
   <si>
     <t>idempleado</t>
   </si>
@@ -1322,9 +1322,6 @@
   </si>
   <si>
     <t>Carballo</t>
-  </si>
-  <si>
-    <t>Fern ndez</t>
   </si>
   <si>
     <t>Nava</t>
@@ -3232,8 +3229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="L263" sqref="L263"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3258,7 +3255,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -3302,7 +3299,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
@@ -3314,7 +3311,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J2" s="1">
         <v>2</v>
@@ -3340,7 +3337,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>17</v>
@@ -3352,7 +3349,7 @@
         <v>19</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J3" s="1">
         <v>2</v>
@@ -3378,7 +3375,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>20</v>
@@ -3390,7 +3387,7 @@
         <v>22</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J4" s="1">
         <v>2</v>
@@ -3416,7 +3413,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
@@ -3428,7 +3425,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="J5" s="1">
         <v>2</v>
@@ -3454,7 +3451,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>23</v>
@@ -3466,7 +3463,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J6" s="1">
         <v>2</v>
@@ -3492,7 +3489,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>28</v>
@@ -3504,7 +3501,7 @@
         <v>30</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J7" s="1">
         <v>2</v>
@@ -3530,7 +3527,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>31</v>
@@ -3542,7 +3539,7 @@
         <v>33</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="J8" s="1">
         <v>2</v>
@@ -3580,7 +3577,7 @@
         <v>36</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="J9" s="1">
         <v>2</v>
@@ -3606,7 +3603,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>37</v>
@@ -3618,7 +3615,7 @@
         <v>39</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="J10" s="1">
         <v>2</v>
@@ -3644,7 +3641,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>40</v>
@@ -3656,7 +3653,7 @@
         <v>42</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="J11" s="1">
         <v>2</v>
@@ -3682,7 +3679,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>43</v>
@@ -3694,7 +3691,7 @@
         <v>45</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J12" s="1">
         <v>2</v>
@@ -3720,7 +3717,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>46</v>
@@ -3732,7 +3729,7 @@
         <v>48</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J13" s="1">
         <v>2</v>
@@ -3758,7 +3755,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>49</v>
@@ -3770,7 +3767,7 @@
         <v>51</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="J14" s="1">
         <v>2</v>
@@ -3796,7 +3793,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>52</v>
@@ -3808,7 +3805,7 @@
         <v>54</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J15" s="1">
         <v>2</v>
@@ -3834,7 +3831,7 @@
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>55</v>
@@ -3846,7 +3843,7 @@
         <v>57</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="J16" s="1">
         <v>2</v>
@@ -3872,7 +3869,7 @@
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>58</v>
@@ -3884,7 +3881,7 @@
         <v>60</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J17" s="1">
         <v>2</v>
@@ -3910,7 +3907,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>61</v>
@@ -3922,7 +3919,7 @@
         <v>63</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J18" s="1">
         <v>2</v>
@@ -3948,7 +3945,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>64</v>
@@ -3960,7 +3957,7 @@
         <v>66</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="J19" s="1">
         <v>2</v>
@@ -3998,7 +3995,7 @@
         <v>14</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="J20" s="1">
         <v>2</v>
@@ -4036,7 +4033,7 @@
         <v>69</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="J21" s="1">
         <v>2</v>
@@ -4062,7 +4059,7 @@
         <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>70</v>
@@ -4074,7 +4071,7 @@
         <v>132</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="J22" s="1">
         <v>2</v>
@@ -4100,7 +4097,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>72</v>
@@ -4112,7 +4109,7 @@
         <v>63</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="J23" s="1">
         <v>2</v>
@@ -4138,7 +4135,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>73</v>
@@ -4150,7 +4147,7 @@
         <v>75</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="J24" s="1">
         <v>2</v>
@@ -4176,7 +4173,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>76</v>
@@ -4188,7 +4185,7 @@
         <v>78</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="J25" s="1">
         <v>2</v>
@@ -4214,7 +4211,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>79</v>
@@ -4226,7 +4223,7 @@
         <v>62</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J26" s="1">
         <v>2</v>
@@ -4252,7 +4249,7 @@
         <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>81</v>
@@ -4264,7 +4261,7 @@
         <v>83</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J27" s="1">
         <v>2</v>
@@ -4290,7 +4287,7 @@
         <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>84</v>
@@ -4302,7 +4299,7 @@
         <v>86</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="J28" s="1">
         <v>2</v>
@@ -4328,7 +4325,7 @@
         <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>84</v>
@@ -4340,7 +4337,7 @@
         <v>88</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="J29" s="1">
         <v>2</v>
@@ -4366,7 +4363,7 @@
         <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>84</v>
@@ -4378,7 +4375,7 @@
         <v>90</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J30" s="1">
         <v>2</v>
@@ -4404,7 +4401,7 @@
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>84</v>
@@ -4416,7 +4413,7 @@
         <v>91</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J31" s="1">
         <v>2</v>
@@ -4454,7 +4451,7 @@
         <v>93</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="J32" s="1">
         <v>2</v>
@@ -4492,7 +4489,7 @@
         <v>96</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="J33" s="1">
         <v>2</v>
@@ -4518,7 +4515,7 @@
         <v>11</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>97</v>
@@ -4530,7 +4527,7 @@
         <v>99</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="J34" s="1">
         <v>2</v>
@@ -4556,7 +4553,7 @@
         <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>100</v>
@@ -4568,7 +4565,7 @@
         <v>102</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="J35" s="1">
         <v>2</v>
@@ -4606,7 +4603,7 @@
         <v>105</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J36" s="1">
         <v>2</v>
@@ -4632,7 +4629,7 @@
         <v>11</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>106</v>
@@ -4644,7 +4641,7 @@
         <v>107</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J37" s="1">
         <v>2</v>
@@ -4682,7 +4679,7 @@
         <v>24</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="J38" s="1">
         <v>5</v>
@@ -4708,7 +4705,7 @@
         <v>11</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>110</v>
@@ -4720,7 +4717,7 @@
         <v>112</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="J39" s="1">
         <v>5</v>
@@ -4746,7 +4743,7 @@
         <v>11</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>113</v>
@@ -4758,7 +4755,7 @@
         <v>63</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="J40" s="1">
         <v>5</v>
@@ -4796,7 +4793,7 @@
         <v>57</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="J41" s="1">
         <v>5</v>
@@ -4834,7 +4831,7 @@
         <v>119</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="J42" s="1">
         <v>5</v>
@@ -4860,7 +4857,7 @@
         <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>120</v>
@@ -4872,7 +4869,7 @@
         <v>95</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="J43" s="1">
         <v>5</v>
@@ -4910,7 +4907,7 @@
         <v>122</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="J44" s="1">
         <v>5</v>
@@ -4948,7 +4945,7 @@
         <v>25</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J45" s="1">
         <v>5</v>
@@ -4986,7 +4983,7 @@
         <v>127</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="J46" s="1">
         <v>5</v>
@@ -5024,7 +5021,7 @@
         <v>130</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="J47" s="1">
         <v>5</v>
@@ -5062,7 +5059,7 @@
         <v>133</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="J48" s="1">
         <v>5</v>
@@ -5100,7 +5097,7 @@
         <v>14</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J49" s="1">
         <v>5</v>
@@ -5126,7 +5123,7 @@
         <v>11</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>136</v>
@@ -5138,7 +5135,7 @@
         <v>25</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J50" s="1">
         <v>5</v>
@@ -5176,7 +5173,7 @@
         <v>140</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="J51" s="1">
         <v>5</v>
@@ -5214,7 +5211,7 @@
         <v>142</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="J52" s="1">
         <v>5</v>
@@ -5252,7 +5249,7 @@
         <v>143</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="J53" s="1">
         <v>5</v>
@@ -5287,10 +5284,10 @@
         <v>75</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="J54" s="1">
         <v>5</v>
@@ -5316,7 +5313,7 @@
         <v>11</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>145</v>
@@ -5328,7 +5325,7 @@
         <v>147</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="J55" s="1">
         <v>5</v>
@@ -5366,7 +5363,7 @@
         <v>150</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="J56" s="1">
         <v>5</v>
@@ -5404,7 +5401,7 @@
         <v>152</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="J57" s="1">
         <v>5</v>
@@ -5442,7 +5439,7 @@
         <v>155</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J58" s="1">
         <v>7</v>
@@ -5480,7 +5477,7 @@
         <v>157</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J59" s="1">
         <v>7</v>
@@ -5518,7 +5515,7 @@
         <v>160</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J60" s="1">
         <v>7</v>
@@ -5556,7 +5553,7 @@
         <v>163</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J61" s="1">
         <v>7</v>
@@ -5594,7 +5591,7 @@
         <v>166</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J62" s="1">
         <v>7</v>
@@ -5632,7 +5629,7 @@
         <v>169</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J63" s="1">
         <v>7</v>
@@ -5670,7 +5667,7 @@
         <v>171</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J64" s="1">
         <v>7</v>
@@ -5708,7 +5705,7 @@
         <v>173</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J65" s="1">
         <v>7</v>
@@ -5746,7 +5743,7 @@
         <v>175</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J66" s="1">
         <v>7</v>
@@ -5784,7 +5781,7 @@
         <v>178</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="J67" s="1">
         <v>7</v>
@@ -5822,7 +5819,7 @@
         <v>181</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J68" s="1">
         <v>7</v>
@@ -5860,7 +5857,7 @@
         <v>183</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="J69" s="1">
         <v>7</v>
@@ -5898,7 +5895,7 @@
         <v>185</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J70" s="1">
         <v>7</v>
@@ -5936,7 +5933,7 @@
         <v>155</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J71" s="1">
         <v>7</v>
@@ -5974,7 +5971,7 @@
         <v>189</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="J72" s="1">
         <v>7</v>
@@ -6012,7 +6009,7 @@
         <v>117</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="J73" s="1">
         <v>7</v>
@@ -6050,7 +6047,7 @@
         <v>194</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="J74" s="1">
         <v>7</v>
@@ -6088,7 +6085,7 @@
         <v>44</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="J75" s="1">
         <v>7</v>
@@ -6114,7 +6111,7 @@
         <v>11</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>197</v>
@@ -6126,7 +6123,7 @@
         <v>198</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="J76" s="1">
         <v>7</v>
@@ -6164,7 +6161,7 @@
         <v>200</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="J77" s="1">
         <v>7</v>
@@ -6202,7 +6199,7 @@
         <v>203</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="J78" s="1">
         <v>7</v>
@@ -6240,7 +6237,7 @@
         <v>27</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="J79" s="1">
         <v>7</v>
@@ -6278,7 +6275,7 @@
         <v>206</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="J80" s="1">
         <v>7</v>
@@ -6316,7 +6313,7 @@
         <v>63</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="J81" s="1">
         <v>7</v>
@@ -6354,7 +6351,7 @@
         <v>209</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J82" s="1">
         <v>7</v>
@@ -6392,7 +6389,7 @@
         <v>211</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J83" s="1">
         <v>7</v>
@@ -6430,7 +6427,7 @@
         <v>213</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J84" s="1">
         <v>7</v>
@@ -6468,7 +6465,7 @@
         <v>216</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="J85" s="1">
         <v>7</v>
@@ -6494,7 +6491,7 @@
         <v>11</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>217</v>
@@ -6506,7 +6503,7 @@
         <v>218</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="J86" s="1">
         <v>7</v>
@@ -6532,7 +6529,7 @@
         <v>11</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>219</v>
@@ -6544,7 +6541,7 @@
         <v>220</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="J87" s="1">
         <v>7</v>
@@ -6570,7 +6567,7 @@
         <v>11</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>221</v>
@@ -6579,10 +6576,10 @@
         <v>222</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="J88" s="1">
         <v>7</v>
@@ -6620,7 +6617,7 @@
         <v>63</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="J89" s="1">
         <v>7</v>
@@ -6658,7 +6655,7 @@
         <v>227</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="J90" s="1">
         <v>7</v>
@@ -6696,7 +6693,7 @@
         <v>50</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="J91" s="1">
         <v>7</v>
@@ -6734,7 +6731,7 @@
         <v>27</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J92" s="1">
         <v>7</v>
@@ -6772,7 +6769,7 @@
         <v>233</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="J93" s="1">
         <v>7</v>
@@ -6810,7 +6807,7 @@
         <v>129</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="J94" s="1">
         <v>7</v>
@@ -6848,7 +6845,7 @@
         <v>236</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J95" s="1">
         <v>7</v>
@@ -6874,7 +6871,7 @@
         <v>11</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>237</v>
@@ -6886,7 +6883,7 @@
         <v>239</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="J96" s="1">
         <v>7</v>
@@ -6912,7 +6909,7 @@
         <v>11</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>240</v>
@@ -6924,7 +6921,7 @@
         <v>242</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="J97" s="1">
         <v>7</v>
@@ -6950,7 +6947,7 @@
         <v>11</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>243</v>
@@ -6962,7 +6959,7 @@
         <v>244</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J98" s="1">
         <v>7</v>
@@ -6988,7 +6985,7 @@
         <v>11</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>245</v>
@@ -7000,7 +6997,7 @@
         <v>14</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="J99" s="1">
         <v>7</v>
@@ -7026,7 +7023,7 @@
         <v>11</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>247</v>
@@ -7038,7 +7035,7 @@
         <v>248</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="J100" s="1">
         <v>7</v>
@@ -7076,7 +7073,7 @@
         <v>155</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J101" s="1">
         <v>7</v>
@@ -7114,7 +7111,7 @@
         <v>205</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="J102" s="1">
         <v>7</v>
@@ -7140,7 +7137,7 @@
         <v>11</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>252</v>
@@ -7152,7 +7149,7 @@
         <v>47</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="J103" s="1">
         <v>7</v>
@@ -7190,7 +7187,7 @@
         <v>255</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J104" s="1">
         <v>7</v>
@@ -7228,7 +7225,7 @@
         <v>257</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="J105" s="1">
         <v>7</v>
@@ -7266,7 +7263,7 @@
         <v>260</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="J106" s="1">
         <v>7</v>
@@ -7304,7 +7301,7 @@
         <v>262</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J107" s="1">
         <v>7</v>
@@ -7342,7 +7339,7 @@
         <v>90</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J108" s="1">
         <v>7</v>
@@ -7374,13 +7371,13 @@
         <v>265</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>266</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J109" s="1">
         <v>6</v>
@@ -7406,7 +7403,7 @@
         <v>11</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>267</v>
@@ -7418,7 +7415,7 @@
         <v>48</v>
       </c>
       <c r="I110" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="J110" s="1">
         <v>6</v>
@@ -7444,7 +7441,7 @@
         <v>11</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>269</v>
@@ -7456,7 +7453,7 @@
         <v>270</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="J111" s="1">
         <v>6</v>
@@ -7482,7 +7479,7 @@
         <v>11</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>271</v>
@@ -7494,7 +7491,7 @@
         <v>272</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="J112" s="1">
         <v>6</v>
@@ -7520,7 +7517,7 @@
         <v>11</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>273</v>
@@ -7532,7 +7529,7 @@
         <v>210</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J113" s="1">
         <v>6</v>
@@ -7558,7 +7555,7 @@
         <v>11</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>274</v>
@@ -7570,7 +7567,7 @@
         <v>48</v>
       </c>
       <c r="I114" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J114" s="1">
         <v>6</v>
@@ -7596,7 +7593,7 @@
         <v>11</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>276</v>
@@ -7608,7 +7605,7 @@
         <v>278</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J115" s="1">
         <v>6</v>
@@ -7634,7 +7631,7 @@
         <v>11</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>279</v>
@@ -7646,7 +7643,7 @@
         <v>281</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J116" s="1">
         <v>6</v>
@@ -7684,7 +7681,7 @@
         <v>284</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J117" s="1">
         <v>6</v>
@@ -7722,7 +7719,7 @@
         <v>286</v>
       </c>
       <c r="I118" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J118" s="1">
         <v>6</v>
@@ -7760,7 +7757,7 @@
         <v>288</v>
       </c>
       <c r="I119" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J119" s="1">
         <v>6</v>
@@ -7798,7 +7795,7 @@
         <v>291</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J120" s="1">
         <v>6</v>
@@ -7836,7 +7833,7 @@
         <v>91</v>
       </c>
       <c r="I121" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J121" s="1">
         <v>6</v>
@@ -7874,7 +7871,7 @@
         <v>133</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J122" s="1">
         <v>6</v>
@@ -7912,7 +7909,7 @@
         <v>296</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J123" s="1">
         <v>6</v>
@@ -7950,7 +7947,7 @@
         <v>298</v>
       </c>
       <c r="I124" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J124" s="1">
         <v>6</v>
@@ -7988,7 +7985,7 @@
         <v>22</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J125" s="1">
         <v>6</v>
@@ -8026,7 +8023,7 @@
         <v>124</v>
       </c>
       <c r="I126" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J126" s="1">
         <v>6</v>
@@ -8052,19 +8049,19 @@
         <v>11</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>300</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>191</v>
+        <v>104</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>63</v>
       </c>
       <c r="I127" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J127" s="1">
         <v>6</v>
@@ -8090,7 +8087,7 @@
         <v>11</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>301</v>
@@ -8102,7 +8099,7 @@
         <v>303</v>
       </c>
       <c r="I128" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J128" s="1">
         <v>6</v>
@@ -8140,7 +8137,7 @@
         <v>306</v>
       </c>
       <c r="I129" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J129" s="1">
         <v>6</v>
@@ -8178,7 +8175,7 @@
         <v>309</v>
       </c>
       <c r="I130" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J130" s="1">
         <v>6</v>
@@ -8204,7 +8201,7 @@
         <v>11</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>310</v>
@@ -8216,7 +8213,7 @@
         <v>311</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J131" s="1">
         <v>6</v>
@@ -8254,7 +8251,7 @@
         <v>98</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J132" s="1">
         <v>6</v>
@@ -8292,7 +8289,7 @@
         <v>316</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J133" s="1">
         <v>6</v>
@@ -8330,7 +8327,7 @@
         <v>319</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J134" s="1">
         <v>6</v>
@@ -8368,7 +8365,7 @@
         <v>183</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J135" s="1">
         <v>6</v>
@@ -8406,7 +8403,7 @@
         <v>107</v>
       </c>
       <c r="I136" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J136" s="1">
         <v>6</v>
@@ -8444,7 +8441,7 @@
         <v>326</v>
       </c>
       <c r="I137" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J137" s="1">
         <v>6</v>
@@ -8482,7 +8479,7 @@
         <v>177</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J138" s="1">
         <v>6</v>
@@ -8508,7 +8505,7 @@
         <v>11</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>329</v>
@@ -8520,7 +8517,7 @@
         <v>171</v>
       </c>
       <c r="I139" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J139" s="1">
         <v>6</v>
@@ -8546,7 +8543,7 @@
         <v>11</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>329</v>
@@ -8558,7 +8555,7 @@
         <v>27</v>
       </c>
       <c r="I140" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J140" s="1">
         <v>6</v>
@@ -8584,7 +8581,7 @@
         <v>11</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>331</v>
@@ -8593,10 +8590,10 @@
         <v>168</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I141" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J141" s="1">
         <v>6</v>
@@ -8634,7 +8631,7 @@
         <v>69</v>
       </c>
       <c r="I142" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="J142" s="1">
         <v>6</v>
@@ -8672,7 +8669,7 @@
         <v>333</v>
       </c>
       <c r="I143" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J143" s="1">
         <v>6</v>
@@ -8710,7 +8707,7 @@
         <v>336</v>
       </c>
       <c r="I144" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="J144" s="1">
         <v>6</v>
@@ -8748,7 +8745,7 @@
         <v>338</v>
       </c>
       <c r="I145" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J145" s="1">
         <v>6</v>
@@ -8786,7 +8783,7 @@
         <v>340</v>
       </c>
       <c r="I146" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="J146" s="1">
         <v>6</v>
@@ -8824,7 +8821,7 @@
         <v>303</v>
       </c>
       <c r="I147" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J147" s="1">
         <v>6</v>
@@ -8862,7 +8859,7 @@
         <v>343</v>
       </c>
       <c r="I148" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J148" s="1">
         <v>6</v>
@@ -8900,7 +8897,7 @@
         <v>346</v>
       </c>
       <c r="I149" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J149" s="1">
         <v>6</v>
@@ -8938,7 +8935,7 @@
         <v>117</v>
       </c>
       <c r="I150" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J150" s="1">
         <v>6</v>
@@ -8976,7 +8973,7 @@
         <v>129</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J151" s="1">
         <v>6</v>
@@ -9014,7 +9011,7 @@
         <v>350</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J152" s="1">
         <v>6</v>
@@ -9052,7 +9049,7 @@
         <v>352</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J153" s="1">
         <v>6</v>
@@ -9090,7 +9087,7 @@
         <v>63</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="J154" s="1">
         <v>6</v>
@@ -9128,7 +9125,7 @@
         <v>14</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J155" s="1">
         <v>6</v>
@@ -9166,7 +9163,7 @@
         <v>356</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="J156" s="1">
         <v>6</v>
@@ -9192,7 +9189,7 @@
         <v>11</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>357</v>
@@ -9204,7 +9201,7 @@
         <v>25</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="J157" s="1">
         <v>6</v>
@@ -9242,7 +9239,7 @@
         <v>360</v>
       </c>
       <c r="I158" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="J158" s="1">
         <v>6</v>
@@ -9280,7 +9277,7 @@
         <v>25</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="J159" s="1">
         <v>6</v>
@@ -9318,7 +9315,7 @@
         <v>205</v>
       </c>
       <c r="I160" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="J160" s="1">
         <v>6</v>
@@ -9356,7 +9353,7 @@
         <v>171</v>
       </c>
       <c r="I161" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="J161" s="1">
         <v>6</v>
@@ -9394,7 +9391,7 @@
         <v>364</v>
       </c>
       <c r="I162" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="J162" s="1">
         <v>6</v>
@@ -9420,7 +9417,7 @@
         <v>11</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>365</v>
@@ -9432,7 +9429,7 @@
         <v>366</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="J163" s="1">
         <v>6</v>
@@ -9470,7 +9467,7 @@
         <v>75</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="J164" s="1">
         <v>6</v>
@@ -9508,7 +9505,7 @@
         <v>191</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="J165" s="1">
         <v>6</v>
@@ -9546,7 +9543,7 @@
         <v>286</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="J166" s="1">
         <v>6</v>
@@ -9584,7 +9581,7 @@
         <v>372</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="J167" s="1">
         <v>6</v>
@@ -9610,7 +9607,7 @@
         <v>11</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>373</v>
@@ -9622,7 +9619,7 @@
         <v>375</v>
       </c>
       <c r="I168" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="J168" s="1">
         <v>6</v>
@@ -9648,7 +9645,7 @@
         <v>11</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>376</v>
@@ -9660,7 +9657,7 @@
         <v>104</v>
       </c>
       <c r="I169" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="J169" s="1">
         <v>6</v>
@@ -9695,10 +9692,10 @@
         <v>117</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I170" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="J170" s="1">
         <v>6</v>
@@ -9736,7 +9733,7 @@
         <v>62</v>
       </c>
       <c r="I171" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="J171" s="1">
         <v>6</v>
@@ -9774,7 +9771,7 @@
         <v>366</v>
       </c>
       <c r="I172" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="J172" s="1">
         <v>6</v>
@@ -9812,7 +9809,7 @@
         <v>294</v>
       </c>
       <c r="I173" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="J173" s="1">
         <v>6</v>
@@ -9838,7 +9835,7 @@
         <v>11</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>382</v>
@@ -9850,7 +9847,7 @@
         <v>384</v>
       </c>
       <c r="I174" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="J174" s="1">
         <v>6</v>
@@ -9888,7 +9885,7 @@
         <v>117</v>
       </c>
       <c r="I175" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="J175" s="1">
         <v>6</v>
@@ -9926,7 +9923,7 @@
         <v>389</v>
       </c>
       <c r="I176" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J176" s="1">
         <v>6</v>
@@ -9964,7 +9961,7 @@
         <v>392</v>
       </c>
       <c r="I177" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="J177" s="1">
         <v>6</v>
@@ -9996,13 +9993,13 @@
         <v>320</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H178" s="1" t="s">
         <v>393</v>
       </c>
       <c r="I178" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="J178" s="1">
         <v>6</v>
@@ -10028,7 +10025,7 @@
         <v>11</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>394</v>
@@ -10040,7 +10037,7 @@
         <v>210</v>
       </c>
       <c r="I179" s="2" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="J179" s="1">
         <v>6</v>
@@ -10078,7 +10075,7 @@
         <v>397</v>
       </c>
       <c r="I180" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="J180" s="1">
         <v>6</v>
@@ -10104,7 +10101,7 @@
         <v>11</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>398</v>
@@ -10116,7 +10113,7 @@
         <v>173</v>
       </c>
       <c r="I181" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="J181" s="1">
         <v>6</v>
@@ -10154,7 +10151,7 @@
         <v>400</v>
       </c>
       <c r="I182" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="J182" s="1">
         <v>6</v>
@@ -10192,7 +10189,7 @@
         <v>402</v>
       </c>
       <c r="I183" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="J183" s="1">
         <v>6</v>
@@ -10218,7 +10215,7 @@
         <v>11</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>403</v>
@@ -10230,7 +10227,7 @@
         <v>404</v>
       </c>
       <c r="I184" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="J184" s="1">
         <v>6</v>
@@ -10268,7 +10265,7 @@
         <v>294</v>
       </c>
       <c r="I185" s="2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="J185" s="1">
         <v>6</v>
@@ -10294,7 +10291,7 @@
         <v>11</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>407</v>
@@ -10306,7 +10303,7 @@
         <v>62</v>
       </c>
       <c r="I186" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="J186" s="1">
         <v>6</v>
@@ -10332,7 +10329,7 @@
         <v>11</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>334</v>
@@ -10344,7 +10341,7 @@
         <v>408</v>
       </c>
       <c r="I187" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="J187" s="1">
         <v>6</v>
@@ -10370,7 +10367,7 @@
         <v>11</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>409</v>
@@ -10382,7 +10379,7 @@
         <v>410</v>
       </c>
       <c r="I188" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="J188" s="1">
         <v>6</v>
@@ -10408,7 +10405,7 @@
         <v>411</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>412</v>
@@ -10420,7 +10417,7 @@
         <v>414</v>
       </c>
       <c r="I189" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="J189" s="1">
         <v>6</v>
@@ -10458,7 +10455,7 @@
         <v>416</v>
       </c>
       <c r="I190" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="J190" s="1">
         <v>6</v>
@@ -10484,7 +10481,7 @@
         <v>411</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>417</v>
@@ -10496,7 +10493,7 @@
         <v>386</v>
       </c>
       <c r="I191" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="J191" s="1">
         <v>6</v>
@@ -10522,7 +10519,7 @@
         <v>411</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>418</v>
@@ -10534,7 +10531,7 @@
         <v>419</v>
       </c>
       <c r="I192" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="J192" s="1">
         <v>6</v>
@@ -10560,19 +10557,19 @@
         <v>411</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>420</v>
       </c>
       <c r="G193" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H193" s="1" t="s">
         <v>47</v>
       </c>
       <c r="I193" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="J193" s="1">
         <v>6</v>
@@ -10598,7 +10595,7 @@
         <v>411</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>421</v>
@@ -10610,7 +10607,7 @@
         <v>371</v>
       </c>
       <c r="I194" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="J194" s="1">
         <v>6</v>
@@ -10636,7 +10633,7 @@
         <v>411</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>23</v>
@@ -10648,7 +10645,7 @@
         <v>48</v>
       </c>
       <c r="I195" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="J195" s="1">
         <v>6</v>
@@ -10674,7 +10671,7 @@
         <v>411</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>234</v>
@@ -10686,7 +10683,7 @@
         <v>168</v>
       </c>
       <c r="I196" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="J196" s="1">
         <v>6</v>
@@ -10712,7 +10709,7 @@
         <v>411</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>424</v>
@@ -10724,7 +10721,7 @@
         <v>355</v>
       </c>
       <c r="I197" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="J197" s="1">
         <v>6</v>
@@ -10750,19 +10747,19 @@
         <v>411</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>254</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H198" s="1" t="s">
         <v>425</v>
       </c>
       <c r="I198" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="J198" s="1">
         <v>6</v>
@@ -10788,7 +10785,7 @@
         <v>411</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>426</v>
@@ -10800,7 +10797,7 @@
         <v>63</v>
       </c>
       <c r="I199" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="J199" s="1">
         <v>6</v>
@@ -10826,7 +10823,7 @@
         <v>411</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>427</v>
@@ -10838,7 +10835,7 @@
         <v>428</v>
       </c>
       <c r="I200" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="J200" s="1">
         <v>6</v>
@@ -10864,7 +10861,7 @@
         <v>411</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>429</v>
@@ -10876,7 +10873,7 @@
         <v>62</v>
       </c>
       <c r="I201" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="J201" s="1">
         <v>6</v>
@@ -10914,7 +10911,7 @@
         <v>431</v>
       </c>
       <c r="I202" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="J202" s="1">
         <v>6</v>
@@ -10940,7 +10937,7 @@
         <v>411</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>432</v>
@@ -10952,7 +10949,7 @@
         <v>168</v>
       </c>
       <c r="I203" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="J203" s="1">
         <v>6</v>
@@ -10978,7 +10975,7 @@
         <v>411</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>204</v>
@@ -10990,7 +10987,7 @@
         <v>75</v>
       </c>
       <c r="I204" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J204" s="1">
         <v>6</v>
@@ -11016,7 +11013,7 @@
         <v>411</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>223</v>
@@ -11028,7 +11025,7 @@
         <v>63</v>
       </c>
       <c r="I205" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="J205" s="1">
         <v>6</v>
@@ -11054,19 +11051,19 @@
         <v>411</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>285</v>
       </c>
       <c r="G206" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H206" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="H206" s="1" t="s">
-        <v>435</v>
-      </c>
       <c r="I206" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="J206" s="1">
         <v>8</v>
@@ -11092,10 +11089,10 @@
         <v>411</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G207" s="1" t="s">
         <v>196</v>
@@ -11104,7 +11101,7 @@
         <v>62</v>
       </c>
       <c r="I207" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="J207" s="1">
         <v>8</v>
@@ -11130,19 +11127,19 @@
         <v>411</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F208" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="G208" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="G208" s="1" t="s">
-        <v>438</v>
       </c>
       <c r="H208" s="1" t="s">
         <v>56</v>
       </c>
       <c r="I208" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="J208" s="1">
         <v>8</v>
@@ -11171,7 +11168,7 @@
         <v>12</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G209" s="1" t="s">
         <v>126</v>
@@ -11180,7 +11177,7 @@
         <v>75</v>
       </c>
       <c r="I209" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="J209" s="1">
         <v>8</v>
@@ -11212,13 +11209,13 @@
         <v>243</v>
       </c>
       <c r="G210" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H210" s="1" t="s">
         <v>281</v>
       </c>
       <c r="I210" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="J210" s="1">
         <v>8</v>
@@ -11244,7 +11241,7 @@
         <v>411</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>52</v>
@@ -11256,7 +11253,7 @@
         <v>98</v>
       </c>
       <c r="I211" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="J211" s="1">
         <v>8</v>
@@ -11282,19 +11279,19 @@
         <v>411</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>287</v>
       </c>
       <c r="G212" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H212" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I212" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="J212" s="1">
         <v>8</v>
@@ -11320,7 +11317,7 @@
         <v>411</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>73</v>
@@ -11332,7 +11329,7 @@
         <v>48</v>
       </c>
       <c r="I213" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="J213" s="1">
         <v>8</v>
@@ -11358,10 +11355,10 @@
         <v>411</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G214" s="1" t="s">
         <v>137</v>
@@ -11370,7 +11367,7 @@
         <v>14</v>
       </c>
       <c r="I214" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="J214" s="1">
         <v>8</v>
@@ -11399,16 +11396,16 @@
         <v>12</v>
       </c>
       <c r="F215" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="G215" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="G215" s="1" t="s">
-        <v>444</v>
       </c>
       <c r="H215" s="1" t="s">
         <v>255</v>
       </c>
       <c r="I215" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J215" s="1">
         <v>8</v>
@@ -11437,16 +11434,16 @@
         <v>12</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G216" s="1" t="s">
         <v>345</v>
       </c>
       <c r="H216" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I216" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J216" s="1">
         <v>8</v>
@@ -11472,7 +11469,7 @@
         <v>411</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>158</v>
@@ -11481,10 +11478,10 @@
         <v>215</v>
       </c>
       <c r="H217" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I217" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="J217" s="1">
         <v>8</v>
@@ -11510,19 +11507,19 @@
         <v>411</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G218" s="1" t="s">
         <v>129</v>
       </c>
       <c r="H218" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I218" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J218" s="1">
         <v>8</v>
@@ -11548,7 +11545,7 @@
         <v>411</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>378</v>
@@ -11560,7 +11557,7 @@
         <v>348</v>
       </c>
       <c r="I219" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="J219" s="1">
         <v>8</v>
@@ -11586,19 +11583,19 @@
         <v>411</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F220" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G220" s="1" t="s">
         <v>450</v>
-      </c>
-      <c r="G220" s="1" t="s">
-        <v>451</v>
       </c>
       <c r="H220" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I220" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="J220" s="1">
         <v>8</v>
@@ -11624,10 +11621,10 @@
         <v>411</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G221" s="1" t="s">
         <v>383</v>
@@ -11636,7 +11633,7 @@
         <v>104</v>
       </c>
       <c r="I221" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="J221" s="1">
         <v>8</v>
@@ -11662,19 +11659,19 @@
         <v>411</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F222" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G222" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="G222" s="1" t="s">
-        <v>454</v>
       </c>
       <c r="H222" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I222" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="J222" s="1">
         <v>8</v>
@@ -11700,10 +11697,10 @@
         <v>411</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F223" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G223" s="1" t="s">
         <v>104</v>
@@ -11712,7 +11709,7 @@
         <v>63</v>
       </c>
       <c r="I223" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="J223" s="1">
         <v>8</v>
@@ -11738,19 +11735,19 @@
         <v>411</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F224" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="G224" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="G224" s="1" t="s">
+      <c r="H224" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="H224" s="1" t="s">
-        <v>458</v>
-      </c>
       <c r="I224" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="J224" s="1">
         <v>8</v>
@@ -11776,19 +11773,19 @@
         <v>411</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F225" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G225" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="H225" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="H225" s="1" t="s">
-        <v>460</v>
-      </c>
       <c r="I225" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="J225" s="1">
         <v>8</v>
@@ -11814,19 +11811,19 @@
         <v>411</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F226" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G226" s="1" t="s">
         <v>33</v>
       </c>
       <c r="H226" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I226" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="J226" s="1">
         <v>8</v>
@@ -11852,19 +11849,19 @@
         <v>411</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G227" s="1" t="s">
         <v>350</v>
       </c>
       <c r="H227" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I227" s="2" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="J227" s="1">
         <v>8</v>
@@ -11890,19 +11887,19 @@
         <v>411</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G228" s="1" t="s">
         <v>57</v>
       </c>
       <c r="H228" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I228" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J228" s="1">
         <v>8</v>
@@ -11931,16 +11928,16 @@
         <v>12</v>
       </c>
       <c r="F229" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G229" s="1" t="s">
         <v>173</v>
       </c>
       <c r="H229" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I229" s="2" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="J229" s="1">
         <v>8</v>
@@ -11969,16 +11966,16 @@
         <v>12</v>
       </c>
       <c r="F230" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="G230" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="G230" s="1" t="s">
-        <v>469</v>
       </c>
       <c r="H230" s="1" t="s">
         <v>168</v>
       </c>
       <c r="I230" s="2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="J230" s="1">
         <v>8</v>
@@ -12004,19 +12001,19 @@
         <v>411</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F231" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="G231" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="G231" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="H231" s="1" t="s">
         <v>350</v>
       </c>
       <c r="I231" s="2" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="J231" s="1">
         <v>8</v>
@@ -12042,19 +12039,19 @@
         <v>411</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F232" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G232" s="1" t="s">
         <v>369</v>
       </c>
       <c r="H232" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I232" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="J232" s="1">
         <v>11</v>
@@ -12080,19 +12077,19 @@
         <v>411</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G233" s="1" t="s">
         <v>111</v>
       </c>
       <c r="H233" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I233" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="J233" s="1">
         <v>11</v>
@@ -12118,19 +12115,19 @@
         <v>411</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F234" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="G234" s="1" t="s">
         <v>476</v>
-      </c>
-      <c r="G234" s="1" t="s">
-        <v>477</v>
       </c>
       <c r="H234" s="1" t="s">
         <v>346</v>
       </c>
       <c r="I234" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="J234" s="1">
         <v>11</v>
@@ -12156,19 +12153,19 @@
         <v>411</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F235" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="G235" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="G235" s="1" t="s">
-        <v>479</v>
       </c>
       <c r="H235" s="1" t="s">
         <v>51</v>
       </c>
       <c r="I235" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="J235" s="1">
         <v>11</v>
@@ -12194,19 +12191,19 @@
         <v>411</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G236" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H236" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I236" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="J236" s="1">
         <v>11</v>
@@ -12232,7 +12229,7 @@
         <v>411</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>234</v>
@@ -12244,7 +12241,7 @@
         <v>321</v>
       </c>
       <c r="I237" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="J237" s="1">
         <v>11</v>
@@ -12270,7 +12267,7 @@
         <v>411</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>170</v>
@@ -12282,7 +12279,7 @@
         <v>180</v>
       </c>
       <c r="I238" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="J238" s="1">
         <v>11</v>
@@ -12308,19 +12305,19 @@
         <v>411</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F239" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="G239" s="1" t="s">
         <v>482</v>
-      </c>
-      <c r="G239" s="1" t="s">
-        <v>483</v>
       </c>
       <c r="H239" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I239" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="J239" s="1">
         <v>11</v>
@@ -12346,19 +12343,19 @@
         <v>411</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F240" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="G240" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="H240" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="G240" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="H240" s="1" t="s">
-        <v>485</v>
-      </c>
       <c r="I240" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="J240" s="1">
         <v>11</v>
@@ -12387,16 +12384,16 @@
         <v>12</v>
       </c>
       <c r="F241" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="G241" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="G241" s="1" t="s">
+      <c r="H241" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="H241" s="1" t="s">
-        <v>488</v>
-      </c>
       <c r="I241" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="J241" s="1">
         <v>11</v>
@@ -12422,19 +12419,19 @@
         <v>411</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F242" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="G242" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="G242" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="H242" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I242" s="2" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="J242" s="1">
         <v>11</v>
@@ -12463,16 +12460,16 @@
         <v>12</v>
       </c>
       <c r="F243" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="G243" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="G243" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="H243" s="1" t="s">
         <v>414</v>
       </c>
       <c r="I243" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="J243" s="1">
         <v>11</v>
@@ -12501,16 +12498,16 @@
         <v>12</v>
       </c>
       <c r="F244" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="G244" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="G244" s="1" t="s">
+      <c r="H244" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="H244" s="1" t="s">
-        <v>495</v>
-      </c>
       <c r="I244" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="J244" s="1">
         <v>11</v>
@@ -12536,10 +12533,10 @@
         <v>411</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G245" s="1" t="s">
         <v>63</v>
@@ -12548,7 +12545,7 @@
         <v>238</v>
       </c>
       <c r="I245" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="J245" s="1">
         <v>11</v>
@@ -12574,7 +12571,7 @@
         <v>411</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>204</v>
@@ -12586,7 +12583,7 @@
         <v>63</v>
       </c>
       <c r="I246" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="J246" s="1">
         <v>11</v>
@@ -12615,16 +12612,16 @@
         <v>12</v>
       </c>
       <c r="F247" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="G247" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="G247" s="1" t="s">
+      <c r="H247" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="H247" s="1" t="s">
-        <v>499</v>
-      </c>
       <c r="I247" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J247" s="1">
         <v>11</v>
@@ -12653,16 +12650,16 @@
         <v>12</v>
       </c>
       <c r="F248" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="G248" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="G248" s="1" t="s">
-        <v>501</v>
-      </c>
       <c r="H248" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I248" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="J248" s="1">
         <v>11</v>
@@ -12688,7 +12685,7 @@
         <v>411</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>31</v>
@@ -12700,7 +12697,7 @@
         <v>286</v>
       </c>
       <c r="I249" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="J249" s="1">
         <v>11</v>
@@ -12729,16 +12726,16 @@
         <v>12</v>
       </c>
       <c r="F250" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="G250" s="1" t="s">
         <v>502</v>
-      </c>
-      <c r="G250" s="1" t="s">
-        <v>503</v>
       </c>
       <c r="H250" s="1" t="s">
         <v>244</v>
       </c>
       <c r="I250" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="J250" s="1">
         <v>11</v>
@@ -12767,16 +12764,16 @@
         <v>12</v>
       </c>
       <c r="F251" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G251" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H251" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I251" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="J251" s="1">
         <v>11</v>
@@ -12802,19 +12799,19 @@
         <v>411</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F252" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G252" s="1" t="s">
         <v>414</v>
       </c>
       <c r="H252" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I252" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="J252" s="1">
         <v>11</v>
@@ -12840,19 +12837,19 @@
         <v>11</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F253" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H253" s="1" t="s">
         <v>291</v>
       </c>
       <c r="I253" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="J253" s="1">
         <v>11</v>
@@ -12878,7 +12875,7 @@
         <v>11</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F254" s="1" t="s">
         <v>339</v>
@@ -12890,7 +12887,7 @@
         <v>19</v>
       </c>
       <c r="I254" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="J254" s="1">
         <v>11</v>
@@ -12916,10 +12913,10 @@
         <v>11</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F255" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G255" s="1" t="s">
         <v>154</v>
@@ -12928,7 +12925,7 @@
         <v>57</v>
       </c>
       <c r="I255" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J255" s="1">
         <v>11</v>
@@ -12966,13 +12963,13 @@
         <v>98</v>
       </c>
       <c r="I256" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="J256" s="1">
         <v>22</v>
       </c>
       <c r="K256" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L256" s="1">
         <v>306</v>
@@ -12998,19 +12995,19 @@
         <v>237</v>
       </c>
       <c r="G257" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H257" s="1" t="s">
         <v>169</v>
       </c>
       <c r="I257" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="J257" s="1">
         <v>22</v>
       </c>
       <c r="K257" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L257" s="1">
         <v>307</v>
@@ -13030,25 +13027,25 @@
         <v>11</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F258" s="1" t="s">
         <v>131</v>
       </c>
       <c r="G258" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H258" s="1" t="s">
         <v>296</v>
       </c>
       <c r="I258" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="J258" s="1">
         <v>22</v>
       </c>
       <c r="K258" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L258" s="1">
         <v>308</v>
@@ -13068,7 +13065,7 @@
         <v>11</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>289</v>
@@ -13080,13 +13077,13 @@
         <v>35</v>
       </c>
       <c r="I259" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="J259" s="1">
         <v>22</v>
       </c>
       <c r="K259" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L259" s="1">
         <v>309</v>
@@ -13106,25 +13103,25 @@
         <v>11</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>144</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H260" s="1" t="s">
         <v>205</v>
       </c>
       <c r="I260" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="J260" s="1">
         <v>23</v>
       </c>
       <c r="K260" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L260" s="1">
         <v>255</v>
@@ -13147,22 +13144,22 @@
         <v>12</v>
       </c>
       <c r="F261" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="G261" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="G261" s="1" t="s">
+      <c r="H261" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="H261" s="1" t="s">
-        <v>516</v>
-      </c>
       <c r="I261" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="J261" s="1">
         <v>23</v>
       </c>
       <c r="K261" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L261" s="1">
         <v>256</v>
@@ -13185,22 +13182,22 @@
         <v>12</v>
       </c>
       <c r="F262" s="1" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="G262" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H262" s="1" t="s">
         <v>165</v>
       </c>
       <c r="I262" s="2" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="J262" s="1">
         <v>23</v>
       </c>
       <c r="K262" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L262" s="1">
         <v>257</v>

</xml_diff>